<commit_message>
add product page complete
</commit_message>
<xml_diff>
--- a/I&C Store Instruments.xlsx
+++ b/I&C Store Instruments.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27823"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27726"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://spplbd-my.sharepoint.com/personal/shuvasisdatta_sppl_com_bd/Documents/SPL/Documents/Store Management/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Adnan\Projects\Store Management\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{756F217F-571D-4F54-B838-8EBB07D7BE58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE0AF587-A124-40C4-A28B-1BA01C3D1450}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="601" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,29 +17,19 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">'I&amp;C STORE MANAGEMENT'!$E$6:$I$241</definedName>
+    <definedName name="_xlnm.Print_Titles" localSheetId="0">'I&amp;C STORE MANAGEMENT'!$6:$6</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="414" uniqueCount="385">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="415" uniqueCount="386">
   <si>
     <t>I&amp;C STORE MANAGEMENT</t>
   </si>
@@ -1196,13 +1186,16 @@
   </si>
   <si>
     <t>PROFIBUS CONNECTOR</t>
+  </si>
+  <si>
+    <t>CURRENT STOCK</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1241,7 +1234,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -1264,37 +1257,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1317,24 +1284,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1618,13 +1577,13 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="E3:I294"/>
+  <dimension ref="E3:J294"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A86" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I90" sqref="I90"/>
+    <sheetView tabSelected="1" topLeftCell="A292" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6:J294"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="30" style="3" bestFit="1" customWidth="1"/>
@@ -1632,25 +1591,26 @@
     <col min="7" max="7" width="48.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="31.85546875" style="3" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="11" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="5:9">
-      <c r="E3" s="10" t="s">
+    <row r="3" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E3" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="F3" s="10"/>
-      <c r="G3" s="10"/>
-      <c r="H3" s="10"/>
-      <c r="I3" s="10"/>
-    </row>
-    <row r="4" spans="5:9">
-      <c r="E4" s="10"/>
-      <c r="F4" s="10"/>
-      <c r="G4" s="10"/>
-      <c r="H4" s="10"/>
-      <c r="I4" s="10"/>
-    </row>
-    <row r="6" spans="5:9" ht="15.75">
+      <c r="F3" s="9"/>
+      <c r="G3" s="9"/>
+      <c r="H3" s="9"/>
+      <c r="I3" s="9"/>
+    </row>
+    <row r="4" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E4" s="9"/>
+      <c r="F4" s="9"/>
+      <c r="G4" s="9"/>
+      <c r="H4" s="9"/>
+      <c r="I4" s="9"/>
+    </row>
+    <row r="6" spans="5:10" ht="31.5" x14ac:dyDescent="0.25">
       <c r="E6" s="5" t="s">
         <v>1</v>
       </c>
@@ -1666,9 +1626,12 @@
       <c r="I6" s="6" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="5:9">
-      <c r="E7" s="11" t="s">
+      <c r="J6" s="10" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="7" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E7" s="8" t="s">
         <v>6</v>
       </c>
       <c r="F7" s="7"/>
@@ -1679,9 +1642,10 @@
       <c r="I7" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="5:9">
-      <c r="E8" s="11"/>
+      <c r="J7" s="11"/>
+    </row>
+    <row r="8" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E8" s="8"/>
       <c r="F8" s="7"/>
       <c r="G8" s="2" t="s">
         <v>8</v>
@@ -1690,9 +1654,10 @@
       <c r="I8" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="5:9">
-      <c r="E9" s="11"/>
+      <c r="J8" s="11"/>
+    </row>
+    <row r="9" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E9" s="8"/>
       <c r="F9" s="7"/>
       <c r="G9" s="2" t="s">
         <v>9</v>
@@ -1701,9 +1666,10 @@
       <c r="I9" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="5:9">
-      <c r="E10" s="11"/>
+      <c r="J9" s="11"/>
+    </row>
+    <row r="10" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E10" s="8"/>
       <c r="F10" s="7"/>
       <c r="G10" s="2" t="s">
         <v>10</v>
@@ -1712,9 +1678,10 @@
       <c r="I10" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="11" spans="5:9">
-      <c r="E11" s="11"/>
+      <c r="J10" s="11"/>
+    </row>
+    <row r="11" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E11" s="8"/>
       <c r="F11" s="7"/>
       <c r="G11" s="2" t="s">
         <v>11</v>
@@ -1723,9 +1690,10 @@
       <c r="I11" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="12" spans="5:9">
-      <c r="E12" s="11"/>
+      <c r="J11" s="11"/>
+    </row>
+    <row r="12" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E12" s="8"/>
       <c r="F12" s="7"/>
       <c r="G12" s="2" t="s">
         <v>12</v>
@@ -1734,9 +1702,10 @@
       <c r="I12" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="13" spans="5:9">
-      <c r="E13" s="11"/>
+      <c r="J12" s="11"/>
+    </row>
+    <row r="13" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E13" s="8"/>
       <c r="F13" s="7"/>
       <c r="G13" s="2" t="s">
         <v>13</v>
@@ -1745,9 +1714,10 @@
       <c r="I13" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="14" spans="5:9">
-      <c r="E14" s="11"/>
+      <c r="J13" s="11"/>
+    </row>
+    <row r="14" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E14" s="8"/>
       <c r="F14" s="7"/>
       <c r="G14" s="2" t="s">
         <v>14</v>
@@ -1756,9 +1726,10 @@
       <c r="I14" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="15" spans="5:9">
-      <c r="E15" s="11"/>
+      <c r="J14" s="11"/>
+    </row>
+    <row r="15" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E15" s="8"/>
       <c r="F15" s="7"/>
       <c r="G15" s="2" t="s">
         <v>15</v>
@@ -1767,9 +1738,10 @@
       <c r="I15" s="2">
         <v>7</v>
       </c>
-    </row>
-    <row r="16" spans="5:9">
-      <c r="E16" s="11"/>
+      <c r="J15" s="11"/>
+    </row>
+    <row r="16" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E16" s="8"/>
       <c r="F16" s="7"/>
       <c r="G16" s="2" t="s">
         <v>16</v>
@@ -1778,9 +1750,10 @@
       <c r="I16" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="17" spans="5:9">
-      <c r="E17" s="11"/>
+      <c r="J16" s="11"/>
+    </row>
+    <row r="17" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E17" s="8"/>
       <c r="F17" s="7"/>
       <c r="G17" s="2" t="s">
         <v>17</v>
@@ -1789,9 +1762,10 @@
       <c r="I17" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="18" spans="5:9">
-      <c r="E18" s="11"/>
+      <c r="J17" s="11"/>
+    </row>
+    <row r="18" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E18" s="8"/>
       <c r="F18" s="7"/>
       <c r="G18" s="2" t="s">
         <v>18</v>
@@ -1800,9 +1774,10 @@
       <c r="I18" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="19" spans="5:9">
-      <c r="E19" s="11"/>
+      <c r="J18" s="11"/>
+    </row>
+    <row r="19" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E19" s="8"/>
       <c r="F19" s="7"/>
       <c r="G19" s="2" t="s">
         <v>19</v>
@@ -1811,9 +1786,10 @@
       <c r="I19" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="20" spans="5:9">
-      <c r="E20" s="11"/>
+      <c r="J19" s="11"/>
+    </row>
+    <row r="20" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E20" s="8"/>
       <c r="F20" s="7"/>
       <c r="G20" s="2" t="s">
         <v>20</v>
@@ -1822,9 +1798,10 @@
       <c r="I20" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="21" spans="5:9">
-      <c r="E21" s="11"/>
+      <c r="J20" s="11"/>
+    </row>
+    <row r="21" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E21" s="8"/>
       <c r="F21" s="7"/>
       <c r="G21" s="2" t="s">
         <v>21</v>
@@ -1833,9 +1810,10 @@
       <c r="I21" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="22" spans="5:9">
-      <c r="E22" s="11"/>
+      <c r="J21" s="11"/>
+    </row>
+    <row r="22" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E22" s="8"/>
       <c r="F22" s="7"/>
       <c r="G22" s="2" t="s">
         <v>22</v>
@@ -1844,9 +1822,10 @@
       <c r="I22" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="23" spans="5:9">
-      <c r="E23" s="11"/>
+      <c r="J22" s="11"/>
+    </row>
+    <row r="23" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E23" s="8"/>
       <c r="F23" s="7"/>
       <c r="G23" s="2" t="s">
         <v>23</v>
@@ -1855,9 +1834,10 @@
       <c r="I23" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="24" spans="5:9">
-      <c r="E24" s="11"/>
+      <c r="J23" s="11"/>
+    </row>
+    <row r="24" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E24" s="8"/>
       <c r="F24" s="7"/>
       <c r="G24" s="2" t="s">
         <v>24</v>
@@ -1866,9 +1846,10 @@
       <c r="I24" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="25" spans="5:9">
-      <c r="E25" s="11"/>
+      <c r="J24" s="11"/>
+    </row>
+    <row r="25" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E25" s="8"/>
       <c r="F25" s="7"/>
       <c r="G25" s="2" t="s">
         <v>25</v>
@@ -1877,9 +1858,10 @@
       <c r="I25" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="26" spans="5:9">
-      <c r="E26" s="11"/>
+      <c r="J25" s="11"/>
+    </row>
+    <row r="26" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E26" s="8"/>
       <c r="F26" s="7"/>
       <c r="G26" s="2" t="s">
         <v>26</v>
@@ -1888,9 +1870,10 @@
       <c r="I26" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="27" spans="5:9">
-      <c r="E27" s="11"/>
+      <c r="J26" s="11"/>
+    </row>
+    <row r="27" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E27" s="8"/>
       <c r="F27" s="7"/>
       <c r="G27" s="2" t="s">
         <v>27</v>
@@ -1899,9 +1882,10 @@
       <c r="I27" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="28" spans="5:9">
-      <c r="E28" s="11"/>
+      <c r="J27" s="11"/>
+    </row>
+    <row r="28" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E28" s="8"/>
       <c r="F28" s="7"/>
       <c r="G28" s="2" t="s">
         <v>28</v>
@@ -1910,9 +1894,10 @@
       <c r="I28" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="29" spans="5:9">
-      <c r="E29" s="11"/>
+      <c r="J28" s="11"/>
+    </row>
+    <row r="29" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E29" s="8"/>
       <c r="F29" s="7"/>
       <c r="G29" s="2" t="s">
         <v>29</v>
@@ -1921,9 +1906,10 @@
       <c r="I29" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="30" spans="5:9">
-      <c r="E30" s="11"/>
+      <c r="J29" s="11"/>
+    </row>
+    <row r="30" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E30" s="8"/>
       <c r="F30" s="7"/>
       <c r="G30" s="2" t="s">
         <v>30</v>
@@ -1932,9 +1918,10 @@
       <c r="I30" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="31" spans="5:9">
-      <c r="E31" s="11"/>
+      <c r="J30" s="11"/>
+    </row>
+    <row r="31" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E31" s="8"/>
       <c r="F31" s="7"/>
       <c r="G31" s="2" t="s">
         <v>31</v>
@@ -1943,9 +1930,10 @@
       <c r="I31" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="32" spans="5:9">
-      <c r="E32" s="11"/>
+      <c r="J31" s="11"/>
+    </row>
+    <row r="32" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E32" s="8"/>
       <c r="F32" s="7"/>
       <c r="G32" s="2" t="s">
         <v>32</v>
@@ -1954,9 +1942,10 @@
       <c r="I32" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="33" spans="5:9">
-      <c r="E33" s="11"/>
+      <c r="J32" s="11"/>
+    </row>
+    <row r="33" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E33" s="8"/>
       <c r="F33" s="7"/>
       <c r="G33" s="2" t="s">
         <v>33</v>
@@ -1965,9 +1954,10 @@
       <c r="I33" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="34" spans="5:9">
-      <c r="E34" s="11"/>
+      <c r="J33" s="11"/>
+    </row>
+    <row r="34" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E34" s="8"/>
       <c r="F34" s="7"/>
       <c r="G34" s="2" t="s">
         <v>34</v>
@@ -1976,9 +1966,10 @@
       <c r="I34" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="35" spans="5:9">
-      <c r="E35" s="11"/>
+      <c r="J34" s="11"/>
+    </row>
+    <row r="35" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E35" s="8"/>
       <c r="F35" s="7"/>
       <c r="G35" s="2" t="s">
         <v>35</v>
@@ -1987,9 +1978,10 @@
       <c r="I35" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="36" spans="5:9">
-      <c r="E36" s="11"/>
+      <c r="J35" s="11"/>
+    </row>
+    <row r="36" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E36" s="8"/>
       <c r="F36" s="7"/>
       <c r="G36" s="2" t="s">
         <v>36</v>
@@ -1998,9 +1990,10 @@
       <c r="I36" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="37" spans="5:9">
-      <c r="E37" s="11"/>
+      <c r="J36" s="11"/>
+    </row>
+    <row r="37" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E37" s="8"/>
       <c r="F37" s="7"/>
       <c r="G37" s="2" t="s">
         <v>37</v>
@@ -2009,9 +2002,10 @@
       <c r="I37" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="38" spans="5:9">
-      <c r="E38" s="11"/>
+      <c r="J37" s="11"/>
+    </row>
+    <row r="38" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E38" s="8"/>
       <c r="F38" s="7"/>
       <c r="G38" s="2" t="s">
         <v>38</v>
@@ -2020,9 +2014,10 @@
       <c r="I38" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="39" spans="5:9">
-      <c r="E39" s="11"/>
+      <c r="J38" s="11"/>
+    </row>
+    <row r="39" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E39" s="8"/>
       <c r="F39" s="7"/>
       <c r="G39" s="2" t="s">
         <v>39</v>
@@ -2031,9 +2026,10 @@
       <c r="I39" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="40" spans="5:9">
-      <c r="E40" s="11"/>
+      <c r="J39" s="11"/>
+    </row>
+    <row r="40" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E40" s="8"/>
       <c r="F40" s="7"/>
       <c r="G40" s="2" t="s">
         <v>40</v>
@@ -2042,9 +2038,10 @@
       <c r="I40" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="41" spans="5:9">
-      <c r="E41" s="11"/>
+      <c r="J40" s="11"/>
+    </row>
+    <row r="41" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E41" s="8"/>
       <c r="F41" s="7"/>
       <c r="G41" s="2" t="s">
         <v>41</v>
@@ -2053,9 +2050,10 @@
       <c r="I41" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="42" spans="5:9">
-      <c r="E42" s="11"/>
+      <c r="J41" s="11"/>
+    </row>
+    <row r="42" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E42" s="8"/>
       <c r="F42" s="7"/>
       <c r="G42" s="2" t="s">
         <v>42</v>
@@ -2064,9 +2062,10 @@
       <c r="I42" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="43" spans="5:9">
-      <c r="E43" s="11"/>
+      <c r="J42" s="11"/>
+    </row>
+    <row r="43" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E43" s="8"/>
       <c r="F43" s="7"/>
       <c r="G43" s="2" t="s">
         <v>43</v>
@@ -2075,9 +2074,10 @@
       <c r="I43" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="44" spans="5:9">
-      <c r="E44" s="11"/>
+      <c r="J43" s="11"/>
+    </row>
+    <row r="44" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E44" s="8"/>
       <c r="F44" s="7"/>
       <c r="G44" s="2" t="s">
         <v>44</v>
@@ -2086,9 +2086,10 @@
       <c r="I44" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="45" spans="5:9">
-      <c r="E45" s="11" t="s">
+      <c r="J44" s="11"/>
+    </row>
+    <row r="45" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E45" s="8" t="s">
         <v>45</v>
       </c>
       <c r="F45" s="7"/>
@@ -2099,9 +2100,10 @@
       <c r="I45" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="46" spans="5:9">
-      <c r="E46" s="11"/>
+      <c r="J45" s="11"/>
+    </row>
+    <row r="46" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E46" s="8"/>
       <c r="F46" s="7"/>
       <c r="G46" s="2" t="s">
         <v>47</v>
@@ -2110,9 +2112,10 @@
       <c r="I46" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="47" spans="5:9">
-      <c r="E47" s="11"/>
+      <c r="J46" s="11"/>
+    </row>
+    <row r="47" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E47" s="8"/>
       <c r="F47" s="7"/>
       <c r="G47" s="2" t="s">
         <v>48</v>
@@ -2121,9 +2124,10 @@
       <c r="I47" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="48" spans="5:9">
-      <c r="E48" s="11"/>
+      <c r="J47" s="11"/>
+    </row>
+    <row r="48" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E48" s="8"/>
       <c r="F48" s="7"/>
       <c r="G48" s="2" t="s">
         <v>49</v>
@@ -2132,9 +2136,10 @@
       <c r="I48" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="49" spans="5:9">
-      <c r="E49" s="11"/>
+      <c r="J48" s="11"/>
+    </row>
+    <row r="49" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E49" s="8"/>
       <c r="F49" s="7"/>
       <c r="G49" s="2" t="s">
         <v>50</v>
@@ -2143,9 +2148,10 @@
       <c r="I49" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="50" spans="5:9">
-      <c r="E50" s="11"/>
+      <c r="J49" s="11"/>
+    </row>
+    <row r="50" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E50" s="8"/>
       <c r="F50" s="7"/>
       <c r="G50" s="2" t="s">
         <v>51</v>
@@ -2154,9 +2160,10 @@
       <c r="I50" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="51" spans="5:9">
-      <c r="E51" s="11"/>
+      <c r="J50" s="11"/>
+    </row>
+    <row r="51" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E51" s="8"/>
       <c r="F51" s="7"/>
       <c r="G51" s="2" t="s">
         <v>52</v>
@@ -2165,9 +2172,10 @@
       <c r="I51" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="52" spans="5:9">
-      <c r="E52" s="11"/>
+      <c r="J51" s="11"/>
+    </row>
+    <row r="52" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E52" s="8"/>
       <c r="F52" s="7"/>
       <c r="G52" s="2" t="s">
         <v>53</v>
@@ -2176,9 +2184,10 @@
       <c r="I52" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="53" spans="5:9">
-      <c r="E53" s="11"/>
+      <c r="J52" s="11"/>
+    </row>
+    <row r="53" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E53" s="8"/>
       <c r="F53" s="7"/>
       <c r="G53" s="2" t="s">
         <v>54</v>
@@ -2187,9 +2196,10 @@
       <c r="I53" s="2">
         <v>3</v>
       </c>
-    </row>
-    <row r="54" spans="5:9">
-      <c r="E54" s="11"/>
+      <c r="J53" s="11"/>
+    </row>
+    <row r="54" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E54" s="8"/>
       <c r="F54" s="7"/>
       <c r="G54" s="2" t="s">
         <v>55</v>
@@ -2198,9 +2208,10 @@
       <c r="I54" s="2">
         <v>3</v>
       </c>
-    </row>
-    <row r="55" spans="5:9">
-      <c r="E55" s="11"/>
+      <c r="J54" s="11"/>
+    </row>
+    <row r="55" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E55" s="8"/>
       <c r="F55" s="7"/>
       <c r="G55" s="2" t="s">
         <v>56</v>
@@ -2209,9 +2220,10 @@
       <c r="I55" s="2">
         <v>3</v>
       </c>
-    </row>
-    <row r="56" spans="5:9">
-      <c r="E56" s="11"/>
+      <c r="J55" s="11"/>
+    </row>
+    <row r="56" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E56" s="8"/>
       <c r="F56" s="7"/>
       <c r="G56" s="2" t="s">
         <v>57</v>
@@ -2220,9 +2232,10 @@
       <c r="I56" s="2">
         <v>3</v>
       </c>
-    </row>
-    <row r="57" spans="5:9">
-      <c r="E57" s="11"/>
+      <c r="J56" s="11"/>
+    </row>
+    <row r="57" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E57" s="8"/>
       <c r="F57" s="7"/>
       <c r="G57" s="2" t="s">
         <v>58</v>
@@ -2231,9 +2244,10 @@
       <c r="I57" s="2">
         <v>3</v>
       </c>
-    </row>
-    <row r="58" spans="5:9">
-      <c r="E58" s="11"/>
+      <c r="J57" s="11"/>
+    </row>
+    <row r="58" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E58" s="8"/>
       <c r="F58" s="7"/>
       <c r="G58" s="2" t="s">
         <v>59</v>
@@ -2242,9 +2256,10 @@
       <c r="I58" s="2">
         <v>4</v>
       </c>
-    </row>
-    <row r="59" spans="5:9">
-      <c r="E59" s="11"/>
+      <c r="J58" s="11"/>
+    </row>
+    <row r="59" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E59" s="8"/>
       <c r="F59" s="7"/>
       <c r="G59" s="2" t="s">
         <v>60</v>
@@ -2253,9 +2268,10 @@
       <c r="I59" s="2">
         <v>3</v>
       </c>
-    </row>
-    <row r="60" spans="5:9">
-      <c r="E60" s="11"/>
+      <c r="J59" s="11"/>
+    </row>
+    <row r="60" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E60" s="8"/>
       <c r="F60" s="7"/>
       <c r="G60" s="2" t="s">
         <v>61</v>
@@ -2264,9 +2280,10 @@
       <c r="I60" s="2">
         <v>4</v>
       </c>
-    </row>
-    <row r="61" spans="5:9">
-      <c r="E61" s="11"/>
+      <c r="J60" s="11"/>
+    </row>
+    <row r="61" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E61" s="8"/>
       <c r="F61" s="7"/>
       <c r="G61" s="2" t="s">
         <v>62</v>
@@ -2275,9 +2292,10 @@
       <c r="I61" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="62" spans="5:9">
-      <c r="E62" s="11"/>
+      <c r="J61" s="11"/>
+    </row>
+    <row r="62" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E62" s="8"/>
       <c r="F62" s="7"/>
       <c r="G62" s="2" t="s">
         <v>63</v>
@@ -2286,9 +2304,10 @@
       <c r="I62" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="63" spans="5:9">
-      <c r="E63" s="11"/>
+      <c r="J62" s="11"/>
+    </row>
+    <row r="63" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E63" s="8"/>
       <c r="F63" s="7"/>
       <c r="G63" s="2" t="s">
         <v>64</v>
@@ -2297,9 +2316,10 @@
       <c r="I63" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="64" spans="5:9">
-      <c r="E64" s="11"/>
+      <c r="J63" s="11"/>
+    </row>
+    <row r="64" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E64" s="8"/>
       <c r="F64" s="7"/>
       <c r="G64" s="2" t="s">
         <v>61</v>
@@ -2308,9 +2328,10 @@
       <c r="I64" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="65" spans="5:9">
-      <c r="E65" s="11"/>
+      <c r="J64" s="11"/>
+    </row>
+    <row r="65" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E65" s="8"/>
       <c r="F65" s="7"/>
       <c r="G65" s="2" t="s">
         <v>65</v>
@@ -2319,9 +2340,10 @@
       <c r="I65" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="66" spans="5:9">
-      <c r="E66" s="11" t="s">
+      <c r="J65" s="11"/>
+    </row>
+    <row r="66" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E66" s="8" t="s">
         <v>66</v>
       </c>
       <c r="F66" s="7"/>
@@ -2334,9 +2356,10 @@
       <c r="I66" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="67" spans="5:9">
-      <c r="E67" s="11"/>
+      <c r="J66" s="11"/>
+    </row>
+    <row r="67" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E67" s="8"/>
       <c r="F67" s="7"/>
       <c r="G67" s="2" t="s">
         <v>69</v>
@@ -2345,9 +2368,10 @@
       <c r="I67" s="2">
         <v>4</v>
       </c>
-    </row>
-    <row r="68" spans="5:9">
-      <c r="E68" s="11"/>
+      <c r="J67" s="11"/>
+    </row>
+    <row r="68" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E68" s="8"/>
       <c r="F68" s="7"/>
       <c r="G68" s="2" t="s">
         <v>70</v>
@@ -2358,9 +2382,10 @@
       <c r="I68" s="2">
         <v>2</v>
       </c>
-    </row>
-    <row r="69" spans="5:9">
-      <c r="E69" s="11"/>
+      <c r="J68" s="11"/>
+    </row>
+    <row r="69" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E69" s="8"/>
       <c r="F69" s="7"/>
       <c r="G69" s="2" t="s">
         <v>72</v>
@@ -2371,9 +2396,10 @@
       <c r="I69" s="2">
         <v>22</v>
       </c>
-    </row>
-    <row r="70" spans="5:9">
-      <c r="E70" s="11"/>
+      <c r="J69" s="11"/>
+    </row>
+    <row r="70" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E70" s="8"/>
       <c r="F70" s="7"/>
       <c r="G70" s="2" t="s">
         <v>74</v>
@@ -2384,9 +2410,10 @@
       <c r="I70" s="2">
         <v>22</v>
       </c>
-    </row>
-    <row r="71" spans="5:9">
-      <c r="E71" s="11"/>
+      <c r="J70" s="11"/>
+    </row>
+    <row r="71" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E71" s="8"/>
       <c r="F71" s="7"/>
       <c r="G71" s="2" t="s">
         <v>76</v>
@@ -2397,9 +2424,10 @@
       <c r="I71" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="72" spans="5:9" ht="30">
-      <c r="E72" s="11"/>
+      <c r="J71" s="11"/>
+    </row>
+    <row r="72" spans="5:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="E72" s="8"/>
       <c r="F72" s="7"/>
       <c r="G72" s="2" t="s">
         <v>78</v>
@@ -2410,9 +2438,10 @@
       <c r="I72" s="2">
         <v>4</v>
       </c>
-    </row>
-    <row r="73" spans="5:9" ht="30">
-      <c r="E73" s="11"/>
+      <c r="J72" s="11"/>
+    </row>
+    <row r="73" spans="5:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="E73" s="8"/>
       <c r="F73" s="7"/>
       <c r="G73" s="2" t="s">
         <v>80</v>
@@ -2423,9 +2452,10 @@
       <c r="I73" s="2">
         <v>2</v>
       </c>
-    </row>
-    <row r="74" spans="5:9" ht="30">
-      <c r="E74" s="11"/>
+      <c r="J73" s="11"/>
+    </row>
+    <row r="74" spans="5:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="E74" s="8"/>
       <c r="F74" s="7"/>
       <c r="G74" s="2" t="s">
         <v>82</v>
@@ -2436,9 +2466,10 @@
       <c r="I74" s="2">
         <v>2</v>
       </c>
-    </row>
-    <row r="75" spans="5:9" ht="30">
-      <c r="E75" s="11"/>
+      <c r="J74" s="11"/>
+    </row>
+    <row r="75" spans="5:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="E75" s="8"/>
       <c r="F75" s="7"/>
       <c r="G75" s="2" t="s">
         <v>84</v>
@@ -2449,9 +2480,10 @@
       <c r="I75" s="2">
         <v>2</v>
       </c>
-    </row>
-    <row r="76" spans="5:9" ht="30">
-      <c r="E76" s="11"/>
+      <c r="J75" s="11"/>
+    </row>
+    <row r="76" spans="5:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="E76" s="8"/>
       <c r="F76" s="7"/>
       <c r="G76" s="2" t="s">
         <v>72</v>
@@ -2462,9 +2494,10 @@
       <c r="I76" s="2">
         <v>4</v>
       </c>
-    </row>
-    <row r="77" spans="5:9" ht="30">
-      <c r="E77" s="11"/>
+      <c r="J76" s="11"/>
+    </row>
+    <row r="77" spans="5:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="E77" s="8"/>
       <c r="F77" s="7"/>
       <c r="G77" s="2" t="s">
         <v>74</v>
@@ -2475,9 +2508,10 @@
       <c r="I77" s="2">
         <v>4</v>
       </c>
-    </row>
-    <row r="78" spans="5:9">
-      <c r="E78" s="11"/>
+      <c r="J77" s="11"/>
+    </row>
+    <row r="78" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E78" s="8"/>
       <c r="F78" s="7"/>
       <c r="G78" s="2" t="s">
         <v>88</v>
@@ -2488,9 +2522,10 @@
       <c r="I78" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="79" spans="5:9">
-      <c r="E79" s="11"/>
+      <c r="J78" s="11"/>
+    </row>
+    <row r="79" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E79" s="8"/>
       <c r="F79" s="7"/>
       <c r="G79" s="2" t="s">
         <v>90</v>
@@ -2501,9 +2536,10 @@
       <c r="I79" s="2">
         <v>2</v>
       </c>
-    </row>
-    <row r="80" spans="5:9">
-      <c r="E80" s="11" t="s">
+      <c r="J79" s="11"/>
+    </row>
+    <row r="80" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E80" s="8" t="s">
         <v>92</v>
       </c>
       <c r="F80" s="7"/>
@@ -2514,9 +2550,10 @@
       <c r="I80" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="81" spans="5:9">
-      <c r="E81" s="11"/>
+      <c r="J80" s="11"/>
+    </row>
+    <row r="81" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E81" s="8"/>
       <c r="F81" s="7"/>
       <c r="G81" s="2" t="s">
         <v>94</v>
@@ -2525,9 +2562,10 @@
       <c r="I81" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="82" spans="5:9" ht="30">
-      <c r="E82" s="11"/>
+      <c r="J81" s="11"/>
+    </row>
+    <row r="82" spans="5:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="E82" s="8"/>
       <c r="F82" s="7"/>
       <c r="G82" s="2" t="s">
         <v>95</v>
@@ -2538,9 +2576,10 @@
       <c r="I82" s="2">
         <v>4</v>
       </c>
-    </row>
-    <row r="83" spans="5:9" ht="30">
-      <c r="E83" s="11"/>
+      <c r="J82" s="11"/>
+    </row>
+    <row r="83" spans="5:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="E83" s="8"/>
       <c r="F83" s="7"/>
       <c r="G83" s="2" t="s">
         <v>97</v>
@@ -2551,9 +2590,10 @@
       <c r="I83" s="2">
         <v>4</v>
       </c>
-    </row>
-    <row r="84" spans="5:9" ht="30">
-      <c r="E84" s="11"/>
+      <c r="J83" s="11"/>
+    </row>
+    <row r="84" spans="5:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="E84" s="8"/>
       <c r="F84" s="7"/>
       <c r="G84" s="2" t="s">
         <v>99</v>
@@ -2564,9 +2604,10 @@
       <c r="I84" s="2">
         <v>3</v>
       </c>
-    </row>
-    <row r="85" spans="5:9" ht="30">
-      <c r="E85" s="11"/>
+      <c r="J84" s="11"/>
+    </row>
+    <row r="85" spans="5:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="E85" s="8"/>
       <c r="F85" s="7"/>
       <c r="G85" s="2" t="s">
         <v>101</v>
@@ -2577,9 +2618,10 @@
       <c r="I85" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="86" spans="5:9" ht="30">
-      <c r="E86" s="11"/>
+      <c r="J85" s="11"/>
+    </row>
+    <row r="86" spans="5:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="E86" s="8"/>
       <c r="F86" s="7"/>
       <c r="G86" s="2" t="s">
         <v>103</v>
@@ -2590,9 +2632,10 @@
       <c r="I86" s="2" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="87" spans="5:9" ht="30">
-      <c r="E87" s="11"/>
+      <c r="J86" s="11"/>
+    </row>
+    <row r="87" spans="5:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="E87" s="8"/>
       <c r="F87" s="7"/>
       <c r="G87" s="2" t="s">
         <v>106</v>
@@ -2603,12 +2646,13 @@
       <c r="I87" s="2">
         <v>2</v>
       </c>
-    </row>
-    <row r="88" spans="5:9" ht="30">
-      <c r="E88" s="12" t="s">
+      <c r="J87" s="11"/>
+    </row>
+    <row r="88" spans="5:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="E88" s="8" t="s">
         <v>108</v>
       </c>
-      <c r="F88" s="8"/>
+      <c r="F88" s="7"/>
       <c r="G88" s="2" t="s">
         <v>109</v>
       </c>
@@ -2618,10 +2662,11 @@
       <c r="I88" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="89" spans="5:9" ht="30">
-      <c r="E89" s="13"/>
-      <c r="F89" s="9"/>
+      <c r="J88" s="11"/>
+    </row>
+    <row r="89" spans="5:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="E89" s="8"/>
+      <c r="F89" s="7"/>
       <c r="G89" s="2" t="s">
         <v>111</v>
       </c>
@@ -2631,9 +2676,10 @@
       <c r="I89" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="90" spans="5:9" ht="30">
-      <c r="E90" s="11" t="s">
+      <c r="J89" s="11"/>
+    </row>
+    <row r="90" spans="5:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="E90" s="8" t="s">
         <v>113</v>
       </c>
       <c r="F90" s="7"/>
@@ -2646,9 +2692,10 @@
       <c r="I90" s="2">
         <v>2</v>
       </c>
-    </row>
-    <row r="91" spans="5:9">
-      <c r="E91" s="11"/>
+      <c r="J90" s="11"/>
+    </row>
+    <row r="91" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E91" s="8"/>
       <c r="F91" s="7"/>
       <c r="G91" s="2" t="s">
         <v>114</v>
@@ -2659,9 +2706,10 @@
       <c r="I91" s="2">
         <v>2</v>
       </c>
-    </row>
-    <row r="92" spans="5:9">
-      <c r="E92" s="11" t="s">
+      <c r="J91" s="11"/>
+    </row>
+    <row r="92" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E92" s="8" t="s">
         <v>116</v>
       </c>
       <c r="F92" s="7"/>
@@ -2672,9 +2720,10 @@
       <c r="I92" s="2">
         <v>2</v>
       </c>
-    </row>
-    <row r="93" spans="5:9">
-      <c r="E93" s="11"/>
+      <c r="J92" s="11"/>
+    </row>
+    <row r="93" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E93" s="8"/>
       <c r="F93" s="7"/>
       <c r="G93" s="2" t="s">
         <v>118</v>
@@ -2683,9 +2732,10 @@
       <c r="I93" s="2">
         <v>3</v>
       </c>
-    </row>
-    <row r="94" spans="5:9">
-      <c r="E94" s="11"/>
+      <c r="J93" s="11"/>
+    </row>
+    <row r="94" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E94" s="8"/>
       <c r="F94" s="7"/>
       <c r="G94" s="2" t="s">
         <v>119</v>
@@ -2694,9 +2744,10 @@
       <c r="I94" s="2">
         <v>5</v>
       </c>
-    </row>
-    <row r="95" spans="5:9">
-      <c r="E95" s="11"/>
+      <c r="J94" s="11"/>
+    </row>
+    <row r="95" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E95" s="8"/>
       <c r="F95" s="7"/>
       <c r="G95" s="2" t="s">
         <v>120</v>
@@ -2705,9 +2756,10 @@
       <c r="I95" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="96" spans="5:9">
-      <c r="E96" s="11"/>
+      <c r="J95" s="11"/>
+    </row>
+    <row r="96" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E96" s="8"/>
       <c r="F96" s="7"/>
       <c r="G96" s="2" t="s">
         <v>121</v>
@@ -2716,9 +2768,10 @@
       <c r="I96" s="2">
         <v>5</v>
       </c>
-    </row>
-    <row r="97" spans="5:9">
-      <c r="E97" s="11"/>
+      <c r="J96" s="11"/>
+    </row>
+    <row r="97" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E97" s="8"/>
       <c r="F97" s="7"/>
       <c r="G97" s="2" t="s">
         <v>122</v>
@@ -2727,9 +2780,10 @@
       <c r="I97" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="98" spans="5:9">
-      <c r="E98" s="11"/>
+      <c r="J97" s="11"/>
+    </row>
+    <row r="98" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E98" s="8"/>
       <c r="F98" s="7"/>
       <c r="G98" s="2" t="s">
         <v>123</v>
@@ -2738,9 +2792,10 @@
       <c r="I98" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="99" spans="5:9">
-      <c r="E99" s="11" t="s">
+      <c r="J98" s="11"/>
+    </row>
+    <row r="99" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E99" s="8" t="s">
         <v>124</v>
       </c>
       <c r="F99" s="7"/>
@@ -2751,9 +2806,10 @@
       <c r="I99" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="100" spans="5:9">
-      <c r="E100" s="11"/>
+      <c r="J99" s="11"/>
+    </row>
+    <row r="100" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E100" s="8"/>
       <c r="F100" s="7"/>
       <c r="G100" s="2" t="s">
         <v>126</v>
@@ -2762,9 +2818,10 @@
       <c r="I100" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="101" spans="5:9">
-      <c r="E101" s="11"/>
+      <c r="J100" s="11"/>
+    </row>
+    <row r="101" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E101" s="8"/>
       <c r="F101" s="7"/>
       <c r="G101" s="2" t="s">
         <v>127</v>
@@ -2773,9 +2830,10 @@
       <c r="I101" s="2">
         <v>2</v>
       </c>
-    </row>
-    <row r="102" spans="5:9">
-      <c r="E102" s="11"/>
+      <c r="J101" s="11"/>
+    </row>
+    <row r="102" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E102" s="8"/>
       <c r="F102" s="7"/>
       <c r="G102" s="2" t="s">
         <v>128</v>
@@ -2784,9 +2842,10 @@
       <c r="I102" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="103" spans="5:9">
-      <c r="E103" s="11"/>
+      <c r="J102" s="11"/>
+    </row>
+    <row r="103" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E103" s="8"/>
       <c r="F103" s="7"/>
       <c r="G103" s="2" t="s">
         <v>129</v>
@@ -2795,9 +2854,10 @@
       <c r="I103" s="2">
         <v>3</v>
       </c>
-    </row>
-    <row r="104" spans="5:9">
-      <c r="E104" s="11"/>
+      <c r="J103" s="11"/>
+    </row>
+    <row r="104" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E104" s="8"/>
       <c r="F104" s="7"/>
       <c r="G104" s="2" t="s">
         <v>130</v>
@@ -2806,9 +2866,10 @@
       <c r="I104" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="105" spans="5:9">
-      <c r="E105" s="11"/>
+      <c r="J104" s="11"/>
+    </row>
+    <row r="105" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E105" s="8"/>
       <c r="F105" s="7"/>
       <c r="G105" s="2" t="s">
         <v>131</v>
@@ -2817,9 +2878,10 @@
       <c r="I105" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="106" spans="5:9">
-      <c r="E106" s="11"/>
+      <c r="J105" s="11"/>
+    </row>
+    <row r="106" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E106" s="8"/>
       <c r="F106" s="7"/>
       <c r="G106" s="2" t="s">
         <v>132</v>
@@ -2828,9 +2890,10 @@
       <c r="I106" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="107" spans="5:9">
-      <c r="E107" s="11"/>
+      <c r="J106" s="11"/>
+    </row>
+    <row r="107" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E107" s="8"/>
       <c r="F107" s="7"/>
       <c r="G107" s="2" t="s">
         <v>133</v>
@@ -2839,9 +2902,10 @@
       <c r="I107" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="108" spans="5:9">
-      <c r="E108" s="11"/>
+      <c r="J107" s="11"/>
+    </row>
+    <row r="108" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E108" s="8"/>
       <c r="F108" s="7"/>
       <c r="G108" s="2" t="s">
         <v>134</v>
@@ -2850,9 +2914,10 @@
       <c r="I108" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="109" spans="5:9">
-      <c r="E109" s="11"/>
+      <c r="J108" s="11"/>
+    </row>
+    <row r="109" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E109" s="8"/>
       <c r="F109" s="7"/>
       <c r="G109" s="2" t="s">
         <v>135</v>
@@ -2861,9 +2926,10 @@
       <c r="I109" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="110" spans="5:9">
-      <c r="E110" s="11"/>
+      <c r="J109" s="11"/>
+    </row>
+    <row r="110" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E110" s="8"/>
       <c r="F110" s="7"/>
       <c r="G110" s="2" t="s">
         <v>136</v>
@@ -2872,9 +2938,10 @@
       <c r="I110" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="111" spans="5:9">
-      <c r="E111" s="11" t="s">
+      <c r="J110" s="11"/>
+    </row>
+    <row r="111" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E111" s="8" t="s">
         <v>137</v>
       </c>
       <c r="F111" s="7"/>
@@ -2885,9 +2952,10 @@
       <c r="I111" s="2">
         <v>2</v>
       </c>
-    </row>
-    <row r="112" spans="5:9">
-      <c r="E112" s="11"/>
+      <c r="J111" s="11"/>
+    </row>
+    <row r="112" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E112" s="8"/>
       <c r="F112" s="7"/>
       <c r="G112" s="2" t="s">
         <v>139</v>
@@ -2896,9 +2964,10 @@
       <c r="I112" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="113" spans="5:9">
-      <c r="E113" s="11"/>
+      <c r="J112" s="11"/>
+    </row>
+    <row r="113" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E113" s="8"/>
       <c r="F113" s="7"/>
       <c r="G113" s="2" t="s">
         <v>140</v>
@@ -2907,9 +2976,10 @@
       <c r="I113" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="114" spans="5:9">
-      <c r="E114" s="11"/>
+      <c r="J113" s="11"/>
+    </row>
+    <row r="114" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E114" s="8"/>
       <c r="F114" s="7"/>
       <c r="G114" s="2" t="s">
         <v>141</v>
@@ -2918,9 +2988,10 @@
       <c r="I114" s="2">
         <v>4</v>
       </c>
-    </row>
-    <row r="115" spans="5:9">
-      <c r="E115" s="11"/>
+      <c r="J114" s="11"/>
+    </row>
+    <row r="115" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E115" s="8"/>
       <c r="F115" s="7"/>
       <c r="G115" s="2" t="s">
         <v>142</v>
@@ -2929,9 +3000,10 @@
       <c r="I115" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="116" spans="5:9">
-      <c r="E116" s="11"/>
+      <c r="J115" s="11"/>
+    </row>
+    <row r="116" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E116" s="8"/>
       <c r="F116" s="7"/>
       <c r="G116" s="2" t="s">
         <v>143</v>
@@ -2940,9 +3012,10 @@
       <c r="I116" s="2">
         <v>2</v>
       </c>
-    </row>
-    <row r="117" spans="5:9">
-      <c r="E117" s="11"/>
+      <c r="J116" s="11"/>
+    </row>
+    <row r="117" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E117" s="8"/>
       <c r="F117" s="7"/>
       <c r="G117" s="2" t="s">
         <v>144</v>
@@ -2951,9 +3024,10 @@
       <c r="I117" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="118" spans="5:9">
-      <c r="E118" s="11"/>
+      <c r="J117" s="11"/>
+    </row>
+    <row r="118" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E118" s="8"/>
       <c r="F118" s="7"/>
       <c r="G118" s="2" t="s">
         <v>145</v>
@@ -2962,9 +3036,10 @@
       <c r="I118" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="119" spans="5:9">
-      <c r="E119" s="11"/>
+      <c r="J118" s="11"/>
+    </row>
+    <row r="119" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E119" s="8"/>
       <c r="F119" s="7"/>
       <c r="G119" s="2" t="s">
         <v>146</v>
@@ -2973,9 +3048,10 @@
       <c r="I119" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="120" spans="5:9">
-      <c r="E120" s="11"/>
+      <c r="J119" s="11"/>
+    </row>
+    <row r="120" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E120" s="8"/>
       <c r="F120" s="7"/>
       <c r="G120" s="2" t="s">
         <v>147</v>
@@ -2984,9 +3060,10 @@
       <c r="I120" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="121" spans="5:9">
-      <c r="E121" s="11" t="s">
+      <c r="J120" s="11"/>
+    </row>
+    <row r="121" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E121" s="8" t="s">
         <v>148</v>
       </c>
       <c r="F121" s="7"/>
@@ -2997,9 +3074,10 @@
       <c r="I121" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="122" spans="5:9">
-      <c r="E122" s="11"/>
+      <c r="J121" s="11"/>
+    </row>
+    <row r="122" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E122" s="8"/>
       <c r="F122" s="7"/>
       <c r="G122" s="2" t="s">
         <v>150</v>
@@ -3008,9 +3086,10 @@
       <c r="I122" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="123" spans="5:9">
-      <c r="E123" s="11"/>
+      <c r="J122" s="11"/>
+    </row>
+    <row r="123" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E123" s="8"/>
       <c r="F123" s="7"/>
       <c r="G123" s="2" t="s">
         <v>151</v>
@@ -3019,9 +3098,10 @@
       <c r="I123" s="2">
         <v>2</v>
       </c>
-    </row>
-    <row r="124" spans="5:9">
-      <c r="E124" s="11"/>
+      <c r="J123" s="11"/>
+    </row>
+    <row r="124" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E124" s="8"/>
       <c r="F124" s="7"/>
       <c r="G124" s="2" t="s">
         <v>152</v>
@@ -3030,9 +3110,10 @@
       <c r="I124" s="2">
         <v>2</v>
       </c>
-    </row>
-    <row r="125" spans="5:9">
-      <c r="E125" s="11"/>
+      <c r="J124" s="11"/>
+    </row>
+    <row r="125" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E125" s="8"/>
       <c r="F125" s="7"/>
       <c r="G125" s="2" t="s">
         <v>153</v>
@@ -3041,9 +3122,10 @@
       <c r="I125" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="126" spans="5:9">
-      <c r="E126" s="11"/>
+      <c r="J125" s="11"/>
+    </row>
+    <row r="126" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E126" s="8"/>
       <c r="F126" s="7"/>
       <c r="G126" s="2" t="s">
         <v>154</v>
@@ -3052,9 +3134,10 @@
       <c r="I126" s="2">
         <v>2</v>
       </c>
-    </row>
-    <row r="127" spans="5:9">
-      <c r="E127" s="11"/>
+      <c r="J126" s="11"/>
+    </row>
+    <row r="127" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E127" s="8"/>
       <c r="F127" s="7"/>
       <c r="G127" s="2" t="s">
         <v>155</v>
@@ -3063,9 +3146,10 @@
       <c r="I127" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="128" spans="5:9">
-      <c r="E128" s="11"/>
+      <c r="J127" s="11"/>
+    </row>
+    <row r="128" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E128" s="8"/>
       <c r="F128" s="7"/>
       <c r="G128" s="2" t="s">
         <v>156</v>
@@ -3074,8 +3158,9 @@
       <c r="I128" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="129" spans="5:9">
+      <c r="J128" s="11"/>
+    </row>
+    <row r="129" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E129" s="7" t="s">
         <v>157</v>
       </c>
@@ -3087,9 +3172,10 @@
       <c r="I129" s="2">
         <v>4</v>
       </c>
-    </row>
-    <row r="130" spans="5:9">
-      <c r="E130" s="11" t="s">
+      <c r="J129" s="11"/>
+    </row>
+    <row r="130" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E130" s="8" t="s">
         <v>159</v>
       </c>
       <c r="F130" s="7"/>
@@ -3100,9 +3186,10 @@
       <c r="I130" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="131" spans="5:9">
-      <c r="E131" s="11"/>
+      <c r="J130" s="11"/>
+    </row>
+    <row r="131" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E131" s="8"/>
       <c r="F131" s="7"/>
       <c r="G131" s="2" t="s">
         <v>161</v>
@@ -3111,9 +3198,10 @@
       <c r="I131" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="132" spans="5:9">
-      <c r="E132" s="11"/>
+      <c r="J131" s="11"/>
+    </row>
+    <row r="132" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E132" s="8"/>
       <c r="F132" s="7"/>
       <c r="G132" s="2" t="s">
         <v>162</v>
@@ -3122,9 +3210,10 @@
       <c r="I132" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="133" spans="5:9">
-      <c r="E133" s="11"/>
+      <c r="J132" s="11"/>
+    </row>
+    <row r="133" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E133" s="8"/>
       <c r="F133" s="7"/>
       <c r="G133" s="2" t="s">
         <v>163</v>
@@ -3133,9 +3222,10 @@
       <c r="I133" s="2">
         <v>2</v>
       </c>
-    </row>
-    <row r="134" spans="5:9">
-      <c r="E134" s="11"/>
+      <c r="J133" s="11"/>
+    </row>
+    <row r="134" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E134" s="8"/>
       <c r="F134" s="7"/>
       <c r="G134" s="2" t="s">
         <v>164</v>
@@ -3144,9 +3234,10 @@
       <c r="I134" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="135" spans="5:9">
-      <c r="E135" s="11"/>
+      <c r="J134" s="11"/>
+    </row>
+    <row r="135" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E135" s="8"/>
       <c r="F135" s="7"/>
       <c r="G135" s="2" t="s">
         <v>165</v>
@@ -3155,9 +3246,10 @@
       <c r="I135" s="2">
         <v>30</v>
       </c>
-    </row>
-    <row r="136" spans="5:9">
-      <c r="E136" s="11"/>
+      <c r="J135" s="11"/>
+    </row>
+    <row r="136" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E136" s="8"/>
       <c r="F136" s="7"/>
       <c r="G136" s="2" t="s">
         <v>166</v>
@@ -3166,9 +3258,10 @@
       <c r="I136" s="2">
         <v>30</v>
       </c>
-    </row>
-    <row r="137" spans="5:9">
-      <c r="E137" s="11"/>
+      <c r="J136" s="11"/>
+    </row>
+    <row r="137" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E137" s="8"/>
       <c r="F137" s="7"/>
       <c r="G137" s="2" t="s">
         <v>167</v>
@@ -3177,9 +3270,10 @@
       <c r="I137" s="2">
         <v>30</v>
       </c>
-    </row>
-    <row r="138" spans="5:9">
-      <c r="E138" s="11"/>
+      <c r="J137" s="11"/>
+    </row>
+    <row r="138" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E138" s="8"/>
       <c r="F138" s="7"/>
       <c r="G138" s="2" t="s">
         <v>168</v>
@@ -3188,9 +3282,10 @@
       <c r="I138" s="2">
         <v>20</v>
       </c>
-    </row>
-    <row r="139" spans="5:9">
-      <c r="E139" s="11"/>
+      <c r="J138" s="11"/>
+    </row>
+    <row r="139" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E139" s="8"/>
       <c r="F139" s="7"/>
       <c r="G139" s="2" t="s">
         <v>169</v>
@@ -3199,9 +3294,10 @@
       <c r="I139" s="2">
         <v>8</v>
       </c>
-    </row>
-    <row r="140" spans="5:9">
-      <c r="E140" s="11"/>
+      <c r="J139" s="11"/>
+    </row>
+    <row r="140" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E140" s="8"/>
       <c r="F140" s="7"/>
       <c r="G140" s="2" t="s">
         <v>170</v>
@@ -3210,9 +3306,10 @@
       <c r="I140" s="2">
         <v>8</v>
       </c>
-    </row>
-    <row r="141" spans="5:9">
-      <c r="E141" s="11"/>
+      <c r="J140" s="11"/>
+    </row>
+    <row r="141" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E141" s="8"/>
       <c r="F141" s="7"/>
       <c r="G141" s="2" t="s">
         <v>171</v>
@@ -3221,9 +3318,10 @@
       <c r="I141" s="2">
         <v>3</v>
       </c>
-    </row>
-    <row r="142" spans="5:9">
-      <c r="E142" s="11"/>
+      <c r="J141" s="11"/>
+    </row>
+    <row r="142" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E142" s="8"/>
       <c r="F142" s="7"/>
       <c r="G142" s="2" t="s">
         <v>172</v>
@@ -3232,9 +3330,10 @@
       <c r="I142" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="143" spans="5:9">
-      <c r="E143" s="11"/>
+      <c r="J142" s="11"/>
+    </row>
+    <row r="143" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E143" s="8"/>
       <c r="F143" s="7"/>
       <c r="G143" s="2" t="s">
         <v>173</v>
@@ -3243,9 +3342,10 @@
       <c r="I143" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="144" spans="5:9">
-      <c r="E144" s="11"/>
+      <c r="J143" s="11"/>
+    </row>
+    <row r="144" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E144" s="8"/>
       <c r="F144" s="7"/>
       <c r="G144" s="2" t="s">
         <v>174</v>
@@ -3254,9 +3354,10 @@
       <c r="I144" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="145" spans="5:9">
-      <c r="E145" s="11"/>
+      <c r="J144" s="11"/>
+    </row>
+    <row r="145" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E145" s="8"/>
       <c r="F145" s="7"/>
       <c r="G145" s="2" t="s">
         <v>175</v>
@@ -3265,9 +3366,10 @@
       <c r="I145" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="146" spans="5:9">
-      <c r="E146" s="11" t="s">
+      <c r="J145" s="11"/>
+    </row>
+    <row r="146" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E146" s="8" t="s">
         <v>176</v>
       </c>
       <c r="F146" s="7"/>
@@ -3278,9 +3380,10 @@
       <c r="I146" s="2">
         <v>6</v>
       </c>
-    </row>
-    <row r="147" spans="5:9">
-      <c r="E147" s="11"/>
+      <c r="J146" s="11"/>
+    </row>
+    <row r="147" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E147" s="8"/>
       <c r="F147" s="7"/>
       <c r="G147" s="2" t="s">
         <v>178</v>
@@ -3289,9 +3392,10 @@
       <c r="I147" s="2">
         <v>4</v>
       </c>
-    </row>
-    <row r="148" spans="5:9">
-      <c r="E148" s="11"/>
+      <c r="J147" s="11"/>
+    </row>
+    <row r="148" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E148" s="8"/>
       <c r="F148" s="7"/>
       <c r="G148" s="2" t="s">
         <v>179</v>
@@ -3300,9 +3404,10 @@
       <c r="I148" s="2">
         <v>5</v>
       </c>
-    </row>
-    <row r="149" spans="5:9">
-      <c r="E149" s="11"/>
+      <c r="J148" s="11"/>
+    </row>
+    <row r="149" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E149" s="8"/>
       <c r="F149" s="7"/>
       <c r="G149" s="2" t="s">
         <v>180</v>
@@ -3311,9 +3416,10 @@
       <c r="I149" s="2">
         <v>2</v>
       </c>
-    </row>
-    <row r="150" spans="5:9">
-      <c r="E150" s="11"/>
+      <c r="J149" s="11"/>
+    </row>
+    <row r="150" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E150" s="8"/>
       <c r="F150" s="7"/>
       <c r="G150" s="2" t="s">
         <v>181</v>
@@ -3322,9 +3428,10 @@
       <c r="I150" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="151" spans="5:9">
-      <c r="E151" s="11"/>
+      <c r="J150" s="11"/>
+    </row>
+    <row r="151" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E151" s="8"/>
       <c r="F151" s="7"/>
       <c r="G151" s="2" t="s">
         <v>182</v>
@@ -3333,9 +3440,10 @@
       <c r="I151" s="2">
         <v>3</v>
       </c>
-    </row>
-    <row r="152" spans="5:9">
-      <c r="E152" s="11"/>
+      <c r="J151" s="11"/>
+    </row>
+    <row r="152" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E152" s="8"/>
       <c r="F152" s="7"/>
       <c r="G152" s="2" t="s">
         <v>183</v>
@@ -3344,9 +3452,10 @@
       <c r="I152" s="2">
         <v>2</v>
       </c>
-    </row>
-    <row r="153" spans="5:9">
-      <c r="E153" s="11"/>
+      <c r="J152" s="11"/>
+    </row>
+    <row r="153" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E153" s="8"/>
       <c r="F153" s="7"/>
       <c r="G153" s="2" t="s">
         <v>184</v>
@@ -3355,9 +3464,10 @@
       <c r="I153" s="2">
         <v>2</v>
       </c>
-    </row>
-    <row r="154" spans="5:9">
-      <c r="E154" s="11" t="s">
+      <c r="J153" s="11"/>
+    </row>
+    <row r="154" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E154" s="8" t="s">
         <v>185</v>
       </c>
       <c r="F154" s="7"/>
@@ -3368,9 +3478,10 @@
       <c r="I154" s="2">
         <v>9</v>
       </c>
-    </row>
-    <row r="155" spans="5:9">
-      <c r="E155" s="11"/>
+      <c r="J154" s="11"/>
+    </row>
+    <row r="155" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E155" s="8"/>
       <c r="F155" s="7"/>
       <c r="G155" s="2" t="s">
         <v>187</v>
@@ -3379,9 +3490,10 @@
       <c r="I155" s="2">
         <v>2</v>
       </c>
-    </row>
-    <row r="156" spans="5:9">
-      <c r="E156" s="11"/>
+      <c r="J155" s="11"/>
+    </row>
+    <row r="156" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E156" s="8"/>
       <c r="F156" s="7"/>
       <c r="G156" s="2" t="s">
         <v>188</v>
@@ -3390,9 +3502,10 @@
       <c r="I156" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="157" spans="5:9">
-      <c r="E157" s="11"/>
+      <c r="J156" s="11"/>
+    </row>
+    <row r="157" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E157" s="8"/>
       <c r="F157" s="7"/>
       <c r="G157" s="2" t="s">
         <v>189</v>
@@ -3401,9 +3514,10 @@
       <c r="I157" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="158" spans="5:9">
-      <c r="E158" s="11"/>
+      <c r="J157" s="11"/>
+    </row>
+    <row r="158" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E158" s="8"/>
       <c r="F158" s="7"/>
       <c r="G158" s="2" t="s">
         <v>190</v>
@@ -3412,9 +3526,10 @@
       <c r="I158" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="159" spans="5:9">
-      <c r="E159" s="11"/>
+      <c r="J158" s="11"/>
+    </row>
+    <row r="159" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E159" s="8"/>
       <c r="F159" s="7"/>
       <c r="G159" s="2" t="s">
         <v>191</v>
@@ -3423,9 +3538,10 @@
       <c r="I159" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="160" spans="5:9">
-      <c r="E160" s="11"/>
+      <c r="J159" s="11"/>
+    </row>
+    <row r="160" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E160" s="8"/>
       <c r="F160" s="7"/>
       <c r="G160" s="2" t="s">
         <v>192</v>
@@ -3434,9 +3550,10 @@
       <c r="I160" s="2">
         <v>5</v>
       </c>
-    </row>
-    <row r="161" spans="5:9">
-      <c r="E161" s="11"/>
+      <c r="J160" s="11"/>
+    </row>
+    <row r="161" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E161" s="8"/>
       <c r="F161" s="7"/>
       <c r="G161" s="2" t="s">
         <v>193</v>
@@ -3445,9 +3562,10 @@
       <c r="I161" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="162" spans="5:9" ht="30">
-      <c r="E162" s="11"/>
+      <c r="J161" s="11"/>
+    </row>
+    <row r="162" spans="5:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="E162" s="8"/>
       <c r="F162" s="7"/>
       <c r="G162" s="2" t="s">
         <v>194</v>
@@ -3458,9 +3576,10 @@
       <c r="I162" s="2">
         <v>5</v>
       </c>
-    </row>
-    <row r="163" spans="5:9">
-      <c r="E163" s="11"/>
+      <c r="J162" s="11"/>
+    </row>
+    <row r="163" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E163" s="8"/>
       <c r="F163" s="7"/>
       <c r="G163" s="2" t="s">
         <v>196</v>
@@ -3471,9 +3590,10 @@
       <c r="I163" s="2">
         <v>2</v>
       </c>
-    </row>
-    <row r="164" spans="5:9">
-      <c r="E164" s="11"/>
+      <c r="J163" s="11"/>
+    </row>
+    <row r="164" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E164" s="8"/>
       <c r="F164" s="7"/>
       <c r="G164" s="2" t="s">
         <v>198</v>
@@ -3484,9 +3604,10 @@
       <c r="I164" s="2">
         <v>2</v>
       </c>
-    </row>
-    <row r="165" spans="5:9" ht="13.5" customHeight="1">
-      <c r="E165" s="11"/>
+      <c r="J164" s="11"/>
+    </row>
+    <row r="165" spans="5:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E165" s="8"/>
       <c r="F165" s="7"/>
       <c r="G165" s="2" t="s">
         <v>200</v>
@@ -3497,9 +3618,10 @@
       <c r="I165" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="166" spans="5:9">
-      <c r="E166" s="11"/>
+      <c r="J165" s="11"/>
+    </row>
+    <row r="166" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E166" s="8"/>
       <c r="F166" s="7"/>
       <c r="G166" s="2" t="s">
         <v>202</v>
@@ -3510,9 +3632,10 @@
       <c r="I166" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="167" spans="5:9">
-      <c r="E167" s="11"/>
+      <c r="J166" s="11"/>
+    </row>
+    <row r="167" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E167" s="8"/>
       <c r="F167" s="7"/>
       <c r="G167" s="2" t="s">
         <v>203</v>
@@ -3523,9 +3646,10 @@
       <c r="I167" s="2">
         <v>3</v>
       </c>
-    </row>
-    <row r="168" spans="5:9">
-      <c r="E168" s="11"/>
+      <c r="J167" s="11"/>
+    </row>
+    <row r="168" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E168" s="8"/>
       <c r="F168" s="7"/>
       <c r="G168" s="2" t="s">
         <v>204</v>
@@ -3536,9 +3660,10 @@
       <c r="I168" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="169" spans="5:9" ht="45">
-      <c r="E169" s="11"/>
+      <c r="J168" s="11"/>
+    </row>
+    <row r="169" spans="5:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="E169" s="8"/>
       <c r="F169" s="7"/>
       <c r="G169" s="2" t="s">
         <v>205</v>
@@ -3549,9 +3674,10 @@
       <c r="I169" s="2">
         <v>2</v>
       </c>
-    </row>
-    <row r="170" spans="5:9">
-      <c r="E170" s="11"/>
+      <c r="J169" s="11"/>
+    </row>
+    <row r="170" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E170" s="8"/>
       <c r="F170" s="7"/>
       <c r="G170" s="2" t="s">
         <v>207</v>
@@ -3560,9 +3686,10 @@
       <c r="I170" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="171" spans="5:9">
-      <c r="E171" s="11" t="s">
+      <c r="J170" s="11"/>
+    </row>
+    <row r="171" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E171" s="8" t="s">
         <v>208</v>
       </c>
       <c r="F171" s="7"/>
@@ -3573,9 +3700,10 @@
       <c r="I171" s="2">
         <v>25</v>
       </c>
-    </row>
-    <row r="172" spans="5:9">
-      <c r="E172" s="11"/>
+      <c r="J171" s="11"/>
+    </row>
+    <row r="172" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E172" s="8"/>
       <c r="F172" s="7"/>
       <c r="G172" s="2" t="s">
         <v>210</v>
@@ -3584,8 +3712,9 @@
       <c r="I172" s="2">
         <v>25</v>
       </c>
-    </row>
-    <row r="173" spans="5:9">
+      <c r="J172" s="11"/>
+    </row>
+    <row r="173" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E173" s="7" t="s">
         <v>211</v>
       </c>
@@ -3597,9 +3726,10 @@
       <c r="I173" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="174" spans="5:9">
-      <c r="E174" s="11" t="s">
+      <c r="J173" s="11"/>
+    </row>
+    <row r="174" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E174" s="8" t="s">
         <v>213</v>
       </c>
       <c r="F174" s="7"/>
@@ -3610,9 +3740,10 @@
       <c r="I174" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="175" spans="5:9">
-      <c r="E175" s="11"/>
+      <c r="J174" s="11"/>
+    </row>
+    <row r="175" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E175" s="8"/>
       <c r="F175" s="7"/>
       <c r="G175" s="2" t="s">
         <v>215</v>
@@ -3621,9 +3752,10 @@
       <c r="I175" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="176" spans="5:9">
-      <c r="E176" s="11"/>
+      <c r="J175" s="11"/>
+    </row>
+    <row r="176" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E176" s="8"/>
       <c r="F176" s="7"/>
       <c r="G176" s="2" t="s">
         <v>216</v>
@@ -3632,9 +3764,10 @@
       <c r="I176" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="177" spans="5:9">
-      <c r="E177" s="11"/>
+      <c r="J176" s="11"/>
+    </row>
+    <row r="177" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E177" s="8"/>
       <c r="F177" s="7"/>
       <c r="G177" s="2" t="s">
         <v>217</v>
@@ -3643,9 +3776,10 @@
       <c r="I177" s="2">
         <v>2</v>
       </c>
-    </row>
-    <row r="178" spans="5:9">
-      <c r="E178" s="11"/>
+      <c r="J177" s="11"/>
+    </row>
+    <row r="178" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E178" s="8"/>
       <c r="F178" s="7"/>
       <c r="G178" s="2" t="s">
         <v>218</v>
@@ -3654,9 +3788,10 @@
       <c r="I178" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="179" spans="5:9">
-      <c r="E179" s="11" t="s">
+      <c r="J178" s="11"/>
+    </row>
+    <row r="179" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E179" s="8" t="s">
         <v>219</v>
       </c>
       <c r="F179" s="7"/>
@@ -3667,9 +3802,10 @@
       <c r="I179" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="180" spans="5:9">
-      <c r="E180" s="11"/>
+      <c r="J179" s="11"/>
+    </row>
+    <row r="180" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E180" s="8"/>
       <c r="F180" s="7"/>
       <c r="G180" s="2" t="s">
         <v>221</v>
@@ -3680,9 +3816,10 @@
       <c r="I180" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="181" spans="5:9">
-      <c r="E181" s="11"/>
+      <c r="J180" s="11"/>
+    </row>
+    <row r="181" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E181" s="8"/>
       <c r="F181" s="7"/>
       <c r="G181" s="2" t="s">
         <v>223</v>
@@ -3693,9 +3830,10 @@
       <c r="I181" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="182" spans="5:9">
-      <c r="E182" s="11"/>
+      <c r="J181" s="11"/>
+    </row>
+    <row r="182" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E182" s="8"/>
       <c r="F182" s="7"/>
       <c r="G182" s="2" t="s">
         <v>224</v>
@@ -3704,9 +3842,10 @@
       <c r="I182" s="2">
         <v>3</v>
       </c>
-    </row>
-    <row r="183" spans="5:9">
-      <c r="E183" s="11"/>
+      <c r="J182" s="11"/>
+    </row>
+    <row r="183" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E183" s="8"/>
       <c r="F183" s="7"/>
       <c r="G183" s="2" t="s">
         <v>225</v>
@@ -3715,9 +3854,10 @@
       <c r="I183" s="2">
         <v>4</v>
       </c>
-    </row>
-    <row r="184" spans="5:9">
-      <c r="E184" s="11"/>
+      <c r="J183" s="11"/>
+    </row>
+    <row r="184" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E184" s="8"/>
       <c r="F184" s="7"/>
       <c r="G184" s="2" t="s">
         <v>226</v>
@@ -3726,9 +3866,10 @@
       <c r="I184" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="185" spans="5:9">
-      <c r="E185" s="11"/>
+      <c r="J184" s="11"/>
+    </row>
+    <row r="185" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E185" s="8"/>
       <c r="F185" s="7"/>
       <c r="G185" s="2" t="s">
         <v>227</v>
@@ -3737,9 +3878,10 @@
       <c r="I185" s="2">
         <v>2</v>
       </c>
-    </row>
-    <row r="186" spans="5:9">
-      <c r="E186" s="11"/>
+      <c r="J185" s="11"/>
+    </row>
+    <row r="186" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E186" s="8"/>
       <c r="F186" s="7"/>
       <c r="G186" s="2" t="s">
         <v>228</v>
@@ -3748,9 +3890,10 @@
       <c r="I186" s="2">
         <v>2</v>
       </c>
-    </row>
-    <row r="187" spans="5:9">
-      <c r="E187" s="11"/>
+      <c r="J186" s="11"/>
+    </row>
+    <row r="187" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E187" s="8"/>
       <c r="F187" s="7"/>
       <c r="G187" s="2" t="s">
         <v>229</v>
@@ -3759,9 +3902,10 @@
       <c r="I187" s="2">
         <v>3</v>
       </c>
-    </row>
-    <row r="188" spans="5:9">
-      <c r="E188" s="11"/>
+      <c r="J187" s="11"/>
+    </row>
+    <row r="188" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E188" s="8"/>
       <c r="F188" s="7"/>
       <c r="G188" s="2" t="s">
         <v>230</v>
@@ -3772,9 +3916,10 @@
       <c r="I188" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="189" spans="5:9">
-      <c r="E189" s="11"/>
+      <c r="J188" s="11"/>
+    </row>
+    <row r="189" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E189" s="8"/>
       <c r="F189" s="7"/>
       <c r="G189" s="2" t="s">
         <v>232</v>
@@ -3783,9 +3928,10 @@
       <c r="I189" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="190" spans="5:9">
-      <c r="E190" s="11"/>
+      <c r="J189" s="11"/>
+    </row>
+    <row r="190" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E190" s="8"/>
       <c r="F190" s="7"/>
       <c r="G190" s="2" t="s">
         <v>233</v>
@@ -3794,9 +3940,10 @@
       <c r="I190" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="191" spans="5:9">
-      <c r="E191" s="11" t="s">
+      <c r="J190" s="11"/>
+    </row>
+    <row r="191" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E191" s="8" t="s">
         <v>234</v>
       </c>
       <c r="F191" s="7"/>
@@ -3807,9 +3954,10 @@
       <c r="I191" s="2">
         <v>2</v>
       </c>
-    </row>
-    <row r="192" spans="5:9">
-      <c r="E192" s="11"/>
+      <c r="J191" s="11"/>
+    </row>
+    <row r="192" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E192" s="8"/>
       <c r="F192" s="7"/>
       <c r="G192" s="2" t="s">
         <v>236</v>
@@ -3818,9 +3966,10 @@
       <c r="I192" s="2">
         <v>2</v>
       </c>
-    </row>
-    <row r="193" spans="5:9">
-      <c r="E193" s="11"/>
+      <c r="J192" s="11"/>
+    </row>
+    <row r="193" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E193" s="8"/>
       <c r="F193" s="7"/>
       <c r="G193" s="2" t="s">
         <v>237</v>
@@ -3829,18 +3978,20 @@
       <c r="I193" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="194" spans="5:9">
-      <c r="E194" s="11"/>
+      <c r="J193" s="11"/>
+    </row>
+    <row r="194" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E194" s="8"/>
       <c r="F194" s="7"/>
       <c r="G194" s="2" t="s">
         <v>238</v>
       </c>
       <c r="H194" s="7"/>
       <c r="I194" s="2"/>
-    </row>
-    <row r="195" spans="5:9">
-      <c r="E195" s="11" t="s">
+      <c r="J194" s="11"/>
+    </row>
+    <row r="195" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E195" s="8" t="s">
         <v>239</v>
       </c>
       <c r="F195" s="7"/>
@@ -3851,9 +4002,10 @@
       <c r="I195" s="2">
         <v>4</v>
       </c>
-    </row>
-    <row r="196" spans="5:9">
-      <c r="E196" s="11"/>
+      <c r="J195" s="11"/>
+    </row>
+    <row r="196" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E196" s="8"/>
       <c r="F196" s="7"/>
       <c r="G196" s="2" t="s">
         <v>241</v>
@@ -3862,9 +4014,10 @@
       <c r="I196" s="2">
         <v>4</v>
       </c>
-    </row>
-    <row r="197" spans="5:9">
-      <c r="E197" s="11"/>
+      <c r="J196" s="11"/>
+    </row>
+    <row r="197" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E197" s="8"/>
       <c r="F197" s="7"/>
       <c r="G197" s="2" t="s">
         <v>242</v>
@@ -3873,9 +4026,10 @@
       <c r="I197" s="2">
         <v>2</v>
       </c>
-    </row>
-    <row r="198" spans="5:9">
-      <c r="E198" s="11"/>
+      <c r="J197" s="11"/>
+    </row>
+    <row r="198" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E198" s="8"/>
       <c r="F198" s="7"/>
       <c r="G198" s="2" t="s">
         <v>243</v>
@@ -3884,9 +4038,10 @@
       <c r="I198" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="199" spans="5:9">
-      <c r="E199" s="11"/>
+      <c r="J198" s="11"/>
+    </row>
+    <row r="199" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E199" s="8"/>
       <c r="F199" s="7"/>
       <c r="G199" s="2" t="s">
         <v>244</v>
@@ -3895,8 +4050,9 @@
       <c r="I199" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="200" spans="5:9">
+      <c r="J199" s="11"/>
+    </row>
+    <row r="200" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E200" s="7" t="s">
         <v>245</v>
       </c>
@@ -3908,9 +4064,10 @@
       <c r="I200" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="201" spans="5:9">
-      <c r="E201" s="11" t="s">
+      <c r="J200" s="11"/>
+    </row>
+    <row r="201" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E201" s="8" t="s">
         <v>247</v>
       </c>
       <c r="F201" s="7"/>
@@ -3921,9 +4078,10 @@
       <c r="I201" s="2">
         <v>7</v>
       </c>
-    </row>
-    <row r="202" spans="5:9">
-      <c r="E202" s="11"/>
+      <c r="J201" s="11"/>
+    </row>
+    <row r="202" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E202" s="8"/>
       <c r="F202" s="7"/>
       <c r="G202" s="2" t="s">
         <v>249</v>
@@ -3932,9 +4090,10 @@
       <c r="I202" s="2">
         <v>2</v>
       </c>
-    </row>
-    <row r="203" spans="5:9">
-      <c r="E203" s="11"/>
+      <c r="J202" s="11"/>
+    </row>
+    <row r="203" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E203" s="8"/>
       <c r="F203" s="7"/>
       <c r="G203" s="2" t="s">
         <v>250</v>
@@ -3943,9 +4102,10 @@
       <c r="I203" s="2">
         <v>3</v>
       </c>
-    </row>
-    <row r="204" spans="5:9">
-      <c r="E204" s="11"/>
+      <c r="J203" s="11"/>
+    </row>
+    <row r="204" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E204" s="8"/>
       <c r="F204" s="7"/>
       <c r="G204" s="2" t="s">
         <v>251</v>
@@ -3954,9 +4114,10 @@
       <c r="I204" s="2">
         <v>2</v>
       </c>
-    </row>
-    <row r="205" spans="5:9">
-      <c r="E205" s="11" t="s">
+      <c r="J204" s="11"/>
+    </row>
+    <row r="205" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E205" s="8" t="s">
         <v>252</v>
       </c>
       <c r="F205" s="7"/>
@@ -3967,9 +4128,10 @@
       <c r="I205" s="2">
         <v>3</v>
       </c>
-    </row>
-    <row r="206" spans="5:9">
-      <c r="E206" s="11"/>
+      <c r="J205" s="11"/>
+    </row>
+    <row r="206" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E206" s="8"/>
       <c r="F206" s="7"/>
       <c r="G206" s="2" t="s">
         <v>254</v>
@@ -3978,9 +4140,10 @@
       <c r="I206" s="2">
         <v>2</v>
       </c>
-    </row>
-    <row r="207" spans="5:9">
-      <c r="E207" s="11"/>
+      <c r="J206" s="11"/>
+    </row>
+    <row r="207" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E207" s="8"/>
       <c r="F207" s="7"/>
       <c r="G207" s="2" t="s">
         <v>255</v>
@@ -3989,9 +4152,10 @@
       <c r="I207" s="2">
         <v>5</v>
       </c>
-    </row>
-    <row r="208" spans="5:9">
-      <c r="E208" s="11"/>
+      <c r="J207" s="11"/>
+    </row>
+    <row r="208" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E208" s="8"/>
       <c r="F208" s="7"/>
       <c r="G208" s="2" t="s">
         <v>256</v>
@@ -4000,9 +4164,10 @@
       <c r="I208" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="209" spans="5:9">
-      <c r="E209" s="11"/>
+      <c r="J208" s="11"/>
+    </row>
+    <row r="209" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E209" s="8"/>
       <c r="F209" s="7"/>
       <c r="G209" s="2" t="s">
         <v>257</v>
@@ -4011,9 +4176,10 @@
       <c r="I209" s="2">
         <v>3</v>
       </c>
-    </row>
-    <row r="210" spans="5:9">
-      <c r="E210" s="11"/>
+      <c r="J209" s="11"/>
+    </row>
+    <row r="210" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E210" s="8"/>
       <c r="F210" s="7"/>
       <c r="G210" s="2" t="s">
         <v>258</v>
@@ -4022,9 +4188,10 @@
       <c r="I210" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="211" spans="5:9">
-      <c r="E211" s="11" t="s">
+      <c r="J210" s="11"/>
+    </row>
+    <row r="211" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E211" s="8" t="s">
         <v>259</v>
       </c>
       <c r="F211" s="7"/>
@@ -4035,9 +4202,10 @@
       <c r="I211" s="2">
         <v>6</v>
       </c>
-    </row>
-    <row r="212" spans="5:9">
-      <c r="E212" s="11"/>
+      <c r="J211" s="11"/>
+    </row>
+    <row r="212" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E212" s="8"/>
       <c r="F212" s="7"/>
       <c r="G212" s="2" t="s">
         <v>261</v>
@@ -4046,9 +4214,10 @@
       <c r="I212" s="2">
         <v>3</v>
       </c>
-    </row>
-    <row r="213" spans="5:9">
-      <c r="E213" s="11"/>
+      <c r="J212" s="11"/>
+    </row>
+    <row r="213" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E213" s="8"/>
       <c r="F213" s="7"/>
       <c r="G213" s="2" t="s">
         <v>262</v>
@@ -4057,9 +4226,10 @@
       <c r="I213" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="214" spans="5:9">
-      <c r="E214" s="11"/>
+      <c r="J213" s="11"/>
+    </row>
+    <row r="214" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E214" s="8"/>
       <c r="F214" s="7"/>
       <c r="G214" s="2" t="s">
         <v>263</v>
@@ -4068,9 +4238,10 @@
       <c r="I214" s="2">
         <v>3</v>
       </c>
-    </row>
-    <row r="215" spans="5:9">
-      <c r="E215" s="11"/>
+      <c r="J214" s="11"/>
+    </row>
+    <row r="215" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E215" s="8"/>
       <c r="F215" s="7"/>
       <c r="G215" s="2" t="s">
         <v>264</v>
@@ -4079,9 +4250,10 @@
       <c r="I215" s="2">
         <v>3</v>
       </c>
-    </row>
-    <row r="216" spans="5:9">
-      <c r="E216" s="11"/>
+      <c r="J215" s="11"/>
+    </row>
+    <row r="216" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E216" s="8"/>
       <c r="F216" s="7"/>
       <c r="G216" s="2" t="s">
         <v>265</v>
@@ -4090,9 +4262,10 @@
       <c r="I216" s="2">
         <v>2</v>
       </c>
-    </row>
-    <row r="217" spans="5:9">
-      <c r="E217" s="11"/>
+      <c r="J216" s="11"/>
+    </row>
+    <row r="217" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E217" s="8"/>
       <c r="F217" s="7"/>
       <c r="G217" s="2" t="s">
         <v>266</v>
@@ -4101,9 +4274,10 @@
       <c r="I217" s="2">
         <v>5</v>
       </c>
-    </row>
-    <row r="218" spans="5:9">
-      <c r="E218" s="11"/>
+      <c r="J217" s="11"/>
+    </row>
+    <row r="218" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E218" s="8"/>
       <c r="F218" s="7"/>
       <c r="G218" s="2" t="s">
         <v>267</v>
@@ -4112,9 +4286,10 @@
       <c r="I218" s="2">
         <v>3</v>
       </c>
-    </row>
-    <row r="219" spans="5:9">
-      <c r="E219" s="11"/>
+      <c r="J218" s="11"/>
+    </row>
+    <row r="219" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E219" s="8"/>
       <c r="F219" s="7"/>
       <c r="G219" s="2" t="s">
         <v>268</v>
@@ -4123,9 +4298,10 @@
       <c r="I219" s="2">
         <v>2</v>
       </c>
-    </row>
-    <row r="220" spans="5:9">
-      <c r="E220" s="11" t="s">
+      <c r="J219" s="11"/>
+    </row>
+    <row r="220" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E220" s="8" t="s">
         <v>269</v>
       </c>
       <c r="F220" s="7"/>
@@ -4136,9 +4312,10 @@
       <c r="I220" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="221" spans="5:9">
-      <c r="E221" s="11"/>
+      <c r="J220" s="11"/>
+    </row>
+    <row r="221" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E221" s="8"/>
       <c r="F221" s="7"/>
       <c r="G221" s="2" t="s">
         <v>271</v>
@@ -4147,9 +4324,10 @@
       <c r="I221" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="222" spans="5:9">
-      <c r="E222" s="11"/>
+      <c r="J221" s="11"/>
+    </row>
+    <row r="222" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E222" s="8"/>
       <c r="F222" s="7"/>
       <c r="G222" s="2" t="s">
         <v>272</v>
@@ -4158,9 +4336,10 @@
       <c r="I222" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="223" spans="5:9">
-      <c r="E223" s="11"/>
+      <c r="J222" s="11"/>
+    </row>
+    <row r="223" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E223" s="8"/>
       <c r="F223" s="7"/>
       <c r="G223" s="2" t="s">
         <v>273</v>
@@ -4169,9 +4348,10 @@
       <c r="I223" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="224" spans="5:9">
-      <c r="E224" s="11"/>
+      <c r="J223" s="11"/>
+    </row>
+    <row r="224" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E224" s="8"/>
       <c r="F224" s="7"/>
       <c r="G224" s="2" t="s">
         <v>274</v>
@@ -4180,9 +4360,10 @@
       <c r="I224" s="2">
         <v>2</v>
       </c>
-    </row>
-    <row r="225" spans="5:9">
-      <c r="E225" s="11"/>
+      <c r="J224" s="11"/>
+    </row>
+    <row r="225" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E225" s="8"/>
       <c r="F225" s="7"/>
       <c r="G225" s="2" t="s">
         <v>275</v>
@@ -4191,9 +4372,10 @@
       <c r="I225" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="226" spans="5:9">
-      <c r="E226" s="11"/>
+      <c r="J225" s="11"/>
+    </row>
+    <row r="226" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E226" s="8"/>
       <c r="F226" s="7"/>
       <c r="G226" s="2" t="s">
         <v>276</v>
@@ -4202,9 +4384,10 @@
       <c r="I226" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="227" spans="5:9">
-      <c r="E227" s="11"/>
+      <c r="J226" s="11"/>
+    </row>
+    <row r="227" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E227" s="8"/>
       <c r="F227" s="7"/>
       <c r="G227" s="2" t="s">
         <v>277</v>
@@ -4213,9 +4396,10 @@
       <c r="I227" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="228" spans="5:9">
-      <c r="E228" s="11"/>
+      <c r="J227" s="11"/>
+    </row>
+    <row r="228" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E228" s="8"/>
       <c r="F228" s="7"/>
       <c r="G228" s="2" t="s">
         <v>278</v>
@@ -4224,9 +4408,10 @@
       <c r="I228" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="229" spans="5:9">
-      <c r="E229" s="11"/>
+      <c r="J228" s="11"/>
+    </row>
+    <row r="229" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E229" s="8"/>
       <c r="F229" s="7"/>
       <c r="G229" s="2" t="s">
         <v>279</v>
@@ -4235,9 +4420,10 @@
       <c r="I229" s="2">
         <v>9</v>
       </c>
-    </row>
-    <row r="230" spans="5:9">
-      <c r="E230" s="11"/>
+      <c r="J229" s="11"/>
+    </row>
+    <row r="230" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E230" s="8"/>
       <c r="F230" s="7"/>
       <c r="G230" s="2" t="s">
         <v>280</v>
@@ -4246,9 +4432,10 @@
       <c r="I230" s="2">
         <v>2</v>
       </c>
-    </row>
-    <row r="231" spans="5:9">
-      <c r="E231" s="11"/>
+      <c r="J230" s="11"/>
+    </row>
+    <row r="231" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E231" s="8"/>
       <c r="F231" s="7"/>
       <c r="G231" s="2" t="s">
         <v>281</v>
@@ -4257,9 +4444,10 @@
       <c r="I231" s="2">
         <v>32</v>
       </c>
-    </row>
-    <row r="232" spans="5:9">
-      <c r="E232" s="11"/>
+      <c r="J231" s="11"/>
+    </row>
+    <row r="232" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E232" s="8"/>
       <c r="F232" s="7"/>
       <c r="G232" s="2" t="s">
         <v>282</v>
@@ -4268,9 +4456,10 @@
       <c r="I232" s="2">
         <v>5</v>
       </c>
-    </row>
-    <row r="233" spans="5:9">
-      <c r="E233" s="11"/>
+      <c r="J232" s="11"/>
+    </row>
+    <row r="233" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E233" s="8"/>
       <c r="F233" s="7"/>
       <c r="G233" s="2" t="s">
         <v>283</v>
@@ -4279,9 +4468,10 @@
       <c r="I233" s="2">
         <v>3</v>
       </c>
-    </row>
-    <row r="234" spans="5:9">
-      <c r="E234" s="11"/>
+      <c r="J233" s="11"/>
+    </row>
+    <row r="234" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E234" s="8"/>
       <c r="F234" s="7"/>
       <c r="G234" s="2" t="s">
         <v>284</v>
@@ -4290,9 +4480,10 @@
       <c r="I234" s="2">
         <v>8</v>
       </c>
-    </row>
-    <row r="235" spans="5:9">
-      <c r="E235" s="11"/>
+      <c r="J234" s="11"/>
+    </row>
+    <row r="235" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E235" s="8"/>
       <c r="F235" s="7"/>
       <c r="G235" s="2" t="s">
         <v>285</v>
@@ -4301,9 +4492,10 @@
       <c r="I235" s="2">
         <v>10</v>
       </c>
-    </row>
-    <row r="236" spans="5:9">
-      <c r="E236" s="11" t="s">
+      <c r="J235" s="11"/>
+    </row>
+    <row r="236" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E236" s="8" t="s">
         <v>286</v>
       </c>
       <c r="F236" s="7"/>
@@ -4314,9 +4506,10 @@
       <c r="I236" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="237" spans="5:9">
-      <c r="E237" s="11"/>
+      <c r="J236" s="11"/>
+    </row>
+    <row r="237" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E237" s="8"/>
       <c r="F237" s="7"/>
       <c r="G237" s="2" t="s">
         <v>288</v>
@@ -4325,9 +4518,10 @@
       <c r="I237" s="2">
         <v>2</v>
       </c>
-    </row>
-    <row r="238" spans="5:9">
-      <c r="E238" s="11"/>
+      <c r="J237" s="11"/>
+    </row>
+    <row r="238" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E238" s="8"/>
       <c r="F238" s="7"/>
       <c r="G238" s="2" t="s">
         <v>289</v>
@@ -4336,9 +4530,10 @@
       <c r="I238" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="239" spans="5:9">
-      <c r="E239" s="11"/>
+      <c r="J238" s="11"/>
+    </row>
+    <row r="239" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E239" s="8"/>
       <c r="F239" s="7"/>
       <c r="G239" s="2" t="s">
         <v>290</v>
@@ -4347,9 +4542,10 @@
       <c r="I239" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="240" spans="5:9">
-      <c r="E240" s="11"/>
+      <c r="J239" s="11"/>
+    </row>
+    <row r="240" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E240" s="8"/>
       <c r="F240" s="7"/>
       <c r="G240" s="2" t="s">
         <v>291</v>
@@ -4358,9 +4554,10 @@
       <c r="I240" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="241" spans="5:9">
-      <c r="E241" s="11"/>
+      <c r="J240" s="11"/>
+    </row>
+    <row r="241" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E241" s="8"/>
       <c r="F241" s="7"/>
       <c r="G241" s="2" t="s">
         <v>292</v>
@@ -4369,9 +4566,10 @@
       <c r="I241" s="2">
         <v>3</v>
       </c>
-    </row>
-    <row r="242" spans="5:9" ht="30">
-      <c r="E242" s="11" t="s">
+      <c r="J241" s="11"/>
+    </row>
+    <row r="242" spans="5:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="E242" s="8" t="s">
         <v>293</v>
       </c>
       <c r="F242" s="7"/>
@@ -4384,9 +4582,10 @@
       <c r="I242" s="2">
         <v>2</v>
       </c>
-    </row>
-    <row r="243" spans="5:9" ht="30">
-      <c r="E243" s="11"/>
+      <c r="J242" s="11"/>
+    </row>
+    <row r="243" spans="5:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="E243" s="8"/>
       <c r="F243" s="7"/>
       <c r="G243" s="2" t="s">
         <v>296</v>
@@ -4397,9 +4596,10 @@
       <c r="I243" s="2">
         <v>3</v>
       </c>
-    </row>
-    <row r="244" spans="5:9">
-      <c r="E244" s="11" t="s">
+      <c r="J243" s="11"/>
+    </row>
+    <row r="244" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E244" s="8" t="s">
         <v>298</v>
       </c>
       <c r="F244" s="7"/>
@@ -4412,9 +4612,10 @@
       <c r="I244" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="245" spans="5:9" ht="30">
-      <c r="E245" s="11"/>
+      <c r="J244" s="11"/>
+    </row>
+    <row r="245" spans="5:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="E245" s="8"/>
       <c r="F245" s="7"/>
       <c r="G245" s="2" t="s">
         <v>301</v>
@@ -4425,9 +4626,10 @@
       <c r="I245" s="2">
         <v>2</v>
       </c>
-    </row>
-    <row r="246" spans="5:9">
-      <c r="E246" s="11"/>
+      <c r="J245" s="11"/>
+    </row>
+    <row r="246" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E246" s="8"/>
       <c r="F246" s="7"/>
       <c r="G246" s="2" t="s">
         <v>303</v>
@@ -4438,9 +4640,10 @@
       <c r="I246" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="247" spans="5:9">
-      <c r="E247" s="11"/>
+      <c r="J246" s="11"/>
+    </row>
+    <row r="247" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E247" s="8"/>
       <c r="F247" s="7"/>
       <c r="G247" s="2" t="s">
         <v>305</v>
@@ -4451,9 +4654,10 @@
       <c r="I247" s="2">
         <v>2</v>
       </c>
-    </row>
-    <row r="248" spans="5:9">
-      <c r="E248" s="11"/>
+      <c r="J247" s="11"/>
+    </row>
+    <row r="248" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E248" s="8"/>
       <c r="F248" s="7"/>
       <c r="G248" s="2" t="s">
         <v>307</v>
@@ -4464,9 +4668,10 @@
       <c r="I248" s="2">
         <v>2</v>
       </c>
-    </row>
-    <row r="249" spans="5:9">
-      <c r="E249" s="11" t="s">
+      <c r="J248" s="11"/>
+    </row>
+    <row r="249" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E249" s="8" t="s">
         <v>309</v>
       </c>
       <c r="F249" s="7"/>
@@ -4479,9 +4684,10 @@
       <c r="I249" s="2">
         <v>3</v>
       </c>
-    </row>
-    <row r="250" spans="5:9" ht="13.5" customHeight="1">
-      <c r="E250" s="11"/>
+      <c r="J249" s="11"/>
+    </row>
+    <row r="250" spans="5:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E250" s="8"/>
       <c r="F250" s="7"/>
       <c r="G250" s="2" t="s">
         <v>312</v>
@@ -4492,9 +4698,10 @@
       <c r="I250" s="2">
         <v>2</v>
       </c>
-    </row>
-    <row r="251" spans="5:9">
-      <c r="E251" s="11" t="s">
+      <c r="J250" s="11"/>
+    </row>
+    <row r="251" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E251" s="8" t="s">
         <v>314</v>
       </c>
       <c r="F251" s="7"/>
@@ -4507,9 +4714,10 @@
       <c r="I251" s="2">
         <v>117</v>
       </c>
-    </row>
-    <row r="252" spans="5:9" ht="13.5" customHeight="1">
-      <c r="E252" s="11"/>
+      <c r="J251" s="11"/>
+    </row>
+    <row r="252" spans="5:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E252" s="8"/>
       <c r="F252" s="7"/>
       <c r="G252" s="2" t="s">
         <v>317</v>
@@ -4520,9 +4728,10 @@
       <c r="I252" s="2">
         <v>3</v>
       </c>
-    </row>
-    <row r="253" spans="5:9" ht="13.5" customHeight="1">
-      <c r="E253" s="11"/>
+      <c r="J252" s="11"/>
+    </row>
+    <row r="253" spans="5:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E253" s="8"/>
       <c r="F253" s="7"/>
       <c r="G253" s="2" t="s">
         <v>319</v>
@@ -4533,9 +4742,10 @@
       <c r="I253" s="2">
         <v>16</v>
       </c>
-    </row>
-    <row r="254" spans="5:9">
-      <c r="E254" s="11" t="s">
+      <c r="J253" s="11"/>
+    </row>
+    <row r="254" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E254" s="8" t="s">
         <v>321</v>
       </c>
       <c r="F254" s="7"/>
@@ -4548,9 +4758,10 @@
       <c r="I254" s="2">
         <v>2</v>
       </c>
-    </row>
-    <row r="255" spans="5:9" ht="30">
-      <c r="E255" s="11"/>
+      <c r="J254" s="11"/>
+    </row>
+    <row r="255" spans="5:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="E255" s="8"/>
       <c r="F255" s="7"/>
       <c r="G255" s="2" t="s">
         <v>324</v>
@@ -4561,9 +4772,10 @@
       <c r="I255" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="256" spans="5:9">
-      <c r="E256" s="11"/>
+      <c r="J255" s="11"/>
+    </row>
+    <row r="256" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E256" s="8"/>
       <c r="F256" s="7"/>
       <c r="G256" s="2" t="s">
         <v>326</v>
@@ -4574,9 +4786,10 @@
       <c r="I256" s="2">
         <v>2</v>
       </c>
-    </row>
-    <row r="257" spans="5:9" ht="45">
-      <c r="E257" s="11"/>
+      <c r="J256" s="11"/>
+    </row>
+    <row r="257" spans="5:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="E257" s="8"/>
       <c r="F257" s="7"/>
       <c r="G257" s="2" t="s">
         <v>328</v>
@@ -4587,9 +4800,10 @@
       <c r="I257" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="258" spans="5:9" ht="45">
-      <c r="E258" s="11"/>
+      <c r="J257" s="11"/>
+    </row>
+    <row r="258" spans="5:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="E258" s="8"/>
       <c r="F258" s="7"/>
       <c r="G258" s="2" t="s">
         <v>330</v>
@@ -4600,9 +4814,10 @@
       <c r="I258" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="259" spans="5:9" ht="45">
-      <c r="E259" s="11"/>
+      <c r="J258" s="11"/>
+    </row>
+    <row r="259" spans="5:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="E259" s="8"/>
       <c r="F259" s="7"/>
       <c r="G259" s="2" t="s">
         <v>332</v>
@@ -4613,9 +4828,10 @@
       <c r="I259" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="260" spans="5:9" ht="30">
-      <c r="E260" s="11"/>
+      <c r="J259" s="11"/>
+    </row>
+    <row r="260" spans="5:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="E260" s="8"/>
       <c r="F260" s="7"/>
       <c r="G260" s="2" t="s">
         <v>334</v>
@@ -4626,9 +4842,10 @@
       <c r="I260" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="261" spans="5:9" ht="30">
-      <c r="E261" s="11"/>
+      <c r="J260" s="11"/>
+    </row>
+    <row r="261" spans="5:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="E261" s="8"/>
       <c r="F261" s="7"/>
       <c r="G261" s="2" t="s">
         <v>336</v>
@@ -4639,9 +4856,10 @@
       <c r="I261" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="262" spans="5:9">
-      <c r="E262" s="11"/>
+      <c r="J261" s="11"/>
+    </row>
+    <row r="262" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E262" s="8"/>
       <c r="F262" s="7"/>
       <c r="G262" s="2" t="s">
         <v>338</v>
@@ -4652,9 +4870,10 @@
       <c r="I262" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="263" spans="5:9" ht="30">
-      <c r="E263" s="11"/>
+      <c r="J262" s="11"/>
+    </row>
+    <row r="263" spans="5:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="E263" s="8"/>
       <c r="F263" s="7"/>
       <c r="G263" s="2" t="s">
         <v>117</v>
@@ -4665,9 +4884,10 @@
       <c r="I263" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="264" spans="5:9" ht="30">
-      <c r="E264" s="11"/>
+      <c r="J263" s="11"/>
+    </row>
+    <row r="264" spans="5:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="E264" s="8"/>
       <c r="F264" s="7"/>
       <c r="G264" s="2" t="s">
         <v>119</v>
@@ -4678,9 +4898,10 @@
       <c r="I264" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="265" spans="5:9" ht="30">
-      <c r="E265" s="11"/>
+      <c r="J264" s="11"/>
+    </row>
+    <row r="265" spans="5:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="E265" s="8"/>
       <c r="F265" s="7"/>
       <c r="G265" s="2" t="s">
         <v>121</v>
@@ -4691,9 +4912,10 @@
       <c r="I265" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="266" spans="5:9" ht="30">
-      <c r="E266" s="11"/>
+      <c r="J265" s="11"/>
+    </row>
+    <row r="266" spans="5:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="E266" s="8"/>
       <c r="F266" s="7"/>
       <c r="G266" s="2" t="s">
         <v>343</v>
@@ -4704,9 +4926,10 @@
       <c r="I266" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="267" spans="5:9" ht="30">
-      <c r="E267" s="11"/>
+      <c r="J266" s="11"/>
+    </row>
+    <row r="267" spans="5:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="E267" s="8"/>
       <c r="F267" s="7"/>
       <c r="G267" s="2" t="s">
         <v>345</v>
@@ -4717,9 +4940,10 @@
       <c r="I267" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="268" spans="5:9" ht="30">
-      <c r="E268" s="11"/>
+      <c r="J267" s="11"/>
+    </row>
+    <row r="268" spans="5:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="E268" s="8"/>
       <c r="F268" s="7"/>
       <c r="G268" s="2" t="s">
         <v>347</v>
@@ -4730,9 +4954,10 @@
       <c r="I268" s="2">
         <v>3</v>
       </c>
-    </row>
-    <row r="269" spans="5:9" ht="30">
-      <c r="E269" s="11"/>
+      <c r="J268" s="11"/>
+    </row>
+    <row r="269" spans="5:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="E269" s="8"/>
       <c r="F269" s="7"/>
       <c r="G269" s="2" t="s">
         <v>349</v>
@@ -4743,16 +4968,18 @@
       <c r="I269" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="270" spans="5:9">
-      <c r="E270" s="11"/>
+      <c r="J269" s="11"/>
+    </row>
+    <row r="270" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E270" s="8"/>
       <c r="F270" s="7"/>
       <c r="G270" s="2"/>
       <c r="H270" s="7"/>
       <c r="I270" s="2"/>
-    </row>
-    <row r="271" spans="5:9">
-      <c r="E271" s="11" t="s">
+      <c r="J270" s="11"/>
+    </row>
+    <row r="271" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E271" s="8" t="s">
         <v>351</v>
       </c>
       <c r="F271" s="7"/>
@@ -4765,9 +4992,10 @@
       <c r="I271" s="2">
         <v>11</v>
       </c>
-    </row>
-    <row r="272" spans="5:9">
-      <c r="E272" s="11"/>
+      <c r="J271" s="11"/>
+    </row>
+    <row r="272" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E272" s="8"/>
       <c r="F272" s="7"/>
       <c r="G272" s="2" t="s">
         <v>353</v>
@@ -4778,9 +5006,10 @@
       <c r="I272" s="2">
         <v>12</v>
       </c>
-    </row>
-    <row r="273" spans="5:9">
-      <c r="E273" s="11"/>
+      <c r="J272" s="11"/>
+    </row>
+    <row r="273" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E273" s="8"/>
       <c r="F273" s="7"/>
       <c r="G273" s="2" t="s">
         <v>354</v>
@@ -4791,9 +5020,10 @@
       <c r="I273" s="2">
         <v>12</v>
       </c>
-    </row>
-    <row r="274" spans="5:9">
-      <c r="E274" s="11"/>
+      <c r="J273" s="11"/>
+    </row>
+    <row r="274" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E274" s="8"/>
       <c r="F274" s="7"/>
       <c r="G274" s="2" t="s">
         <v>355</v>
@@ -4804,9 +5034,10 @@
       <c r="I274" s="2">
         <v>12</v>
       </c>
-    </row>
-    <row r="275" spans="5:9">
-      <c r="E275" s="11"/>
+      <c r="J274" s="11"/>
+    </row>
+    <row r="275" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E275" s="8"/>
       <c r="F275" s="7"/>
       <c r="G275" s="2" t="s">
         <v>356</v>
@@ -4817,9 +5048,10 @@
       <c r="I275" s="2">
         <v>12</v>
       </c>
-    </row>
-    <row r="276" spans="5:9">
-      <c r="E276" s="11"/>
+      <c r="J275" s="11"/>
+    </row>
+    <row r="276" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E276" s="8"/>
       <c r="F276" s="7"/>
       <c r="G276" s="2" t="s">
         <v>357</v>
@@ -4830,9 +5062,10 @@
       <c r="I276" s="2">
         <v>12</v>
       </c>
-    </row>
-    <row r="277" spans="5:9">
-      <c r="E277" s="11"/>
+      <c r="J276" s="11"/>
+    </row>
+    <row r="277" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E277" s="8"/>
       <c r="F277" s="7"/>
       <c r="G277" s="2" t="s">
         <v>358</v>
@@ -4843,9 +5076,10 @@
       <c r="I277" s="2">
         <v>12</v>
       </c>
-    </row>
-    <row r="278" spans="5:9">
-      <c r="E278" s="11"/>
+      <c r="J277" s="11"/>
+    </row>
+    <row r="278" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E278" s="8"/>
       <c r="F278" s="7"/>
       <c r="G278" s="2" t="s">
         <v>359</v>
@@ -4856,9 +5090,10 @@
       <c r="I278" s="2">
         <v>24</v>
       </c>
-    </row>
-    <row r="279" spans="5:9">
-      <c r="E279" s="11"/>
+      <c r="J278" s="11"/>
+    </row>
+    <row r="279" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E279" s="8"/>
       <c r="F279" s="7"/>
       <c r="G279" s="2" t="s">
         <v>360</v>
@@ -4869,9 +5104,10 @@
       <c r="I279" s="2">
         <v>12</v>
       </c>
-    </row>
-    <row r="280" spans="5:9">
-      <c r="E280" s="11"/>
+      <c r="J279" s="11"/>
+    </row>
+    <row r="280" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E280" s="8"/>
       <c r="F280" s="7"/>
       <c r="G280" s="2" t="s">
         <v>361</v>
@@ -4882,9 +5118,10 @@
       <c r="I280" s="2">
         <v>24</v>
       </c>
-    </row>
-    <row r="281" spans="5:9">
-      <c r="E281" s="11"/>
+      <c r="J280" s="11"/>
+    </row>
+    <row r="281" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E281" s="8"/>
       <c r="F281" s="7"/>
       <c r="G281" s="2" t="s">
         <v>362</v>
@@ -4895,21 +5132,24 @@
       <c r="I281" s="2">
         <v>12</v>
       </c>
-    </row>
-    <row r="282" spans="5:9">
-      <c r="E282" s="11"/>
-      <c r="G282" s="1" t="s">
+      <c r="J281" s="11"/>
+    </row>
+    <row r="282" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E282" s="8"/>
+      <c r="F282" s="7"/>
+      <c r="G282" s="2" t="s">
         <v>363</v>
       </c>
-      <c r="H282" s="1" t="s">
+      <c r="H282" s="2" t="s">
         <v>363</v>
       </c>
       <c r="I282" s="2">
         <v>12</v>
       </c>
-    </row>
-    <row r="283" spans="5:9">
-      <c r="E283" s="11"/>
+      <c r="J282" s="11"/>
+    </row>
+    <row r="283" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E283" s="8"/>
       <c r="F283" s="7"/>
       <c r="G283" s="2" t="s">
         <v>364</v>
@@ -4920,9 +5160,10 @@
       <c r="I283" s="2">
         <v>12</v>
       </c>
-    </row>
-    <row r="284" spans="5:9">
-      <c r="E284" s="11"/>
+      <c r="J283" s="11"/>
+    </row>
+    <row r="284" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E284" s="8"/>
       <c r="F284" s="7"/>
       <c r="G284" s="2" t="s">
         <v>365</v>
@@ -4933,9 +5174,10 @@
       <c r="I284" s="2">
         <v>12</v>
       </c>
-    </row>
-    <row r="285" spans="5:9">
-      <c r="E285" s="11"/>
+      <c r="J284" s="11"/>
+    </row>
+    <row r="285" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E285" s="8"/>
       <c r="F285" s="7"/>
       <c r="G285" s="2" t="s">
         <v>366</v>
@@ -4946,9 +5188,10 @@
       <c r="I285" s="2">
         <v>12</v>
       </c>
-    </row>
-    <row r="286" spans="5:9">
-      <c r="E286" s="11" t="s">
+      <c r="J285" s="11"/>
+    </row>
+    <row r="286" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E286" s="8" t="s">
         <v>367</v>
       </c>
       <c r="F286" s="7"/>
@@ -4961,9 +5204,10 @@
       <c r="I286" s="2">
         <v>82</v>
       </c>
-    </row>
-    <row r="287" spans="5:9">
-      <c r="E287" s="11"/>
+      <c r="J286" s="11"/>
+    </row>
+    <row r="287" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E287" s="8"/>
       <c r="F287" s="7"/>
       <c r="G287" s="2" t="s">
         <v>370</v>
@@ -4974,9 +5218,10 @@
       <c r="I287" s="2">
         <v>182</v>
       </c>
-    </row>
-    <row r="288" spans="5:9">
-      <c r="E288" s="11"/>
+      <c r="J287" s="11"/>
+    </row>
+    <row r="288" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E288" s="8"/>
       <c r="F288" s="7"/>
       <c r="G288" s="2" t="s">
         <v>371</v>
@@ -4987,9 +5232,10 @@
       <c r="I288" s="2">
         <v>91</v>
       </c>
-    </row>
-    <row r="289" spans="5:9" ht="45">
-      <c r="E289" s="11" t="s">
+      <c r="J288" s="11"/>
+    </row>
+    <row r="289" spans="5:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="E289" s="8" t="s">
         <v>372</v>
       </c>
       <c r="F289" s="7"/>
@@ -5002,9 +5248,10 @@
       <c r="I289" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="290" spans="5:9" ht="45">
-      <c r="E290" s="11"/>
+      <c r="J289" s="11"/>
+    </row>
+    <row r="290" spans="5:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="E290" s="8"/>
       <c r="F290" s="7"/>
       <c r="G290" s="2" t="s">
         <v>375</v>
@@ -5015,9 +5262,10 @@
       <c r="I290" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="291" spans="5:9" ht="30">
-      <c r="E291" s="11"/>
+      <c r="J290" s="11"/>
+    </row>
+    <row r="291" spans="5:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="E291" s="8"/>
       <c r="F291" s="7"/>
       <c r="G291" s="2" t="s">
         <v>377</v>
@@ -5028,9 +5276,10 @@
       <c r="I291" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="292" spans="5:9" ht="30">
-      <c r="E292" s="11"/>
+      <c r="J291" s="11"/>
+    </row>
+    <row r="292" spans="5:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="E292" s="8"/>
       <c r="F292" s="7"/>
       <c r="G292" s="2" t="s">
         <v>379</v>
@@ -5041,9 +5290,10 @@
       <c r="I292" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="293" spans="5:9" ht="30">
-      <c r="E293" s="11"/>
+      <c r="J292" s="11"/>
+    </row>
+    <row r="293" spans="5:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="E293" s="8"/>
       <c r="F293" s="7"/>
       <c r="G293" s="2" t="s">
         <v>381</v>
@@ -5054,9 +5304,10 @@
       <c r="I293" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="294" spans="5:9">
-      <c r="E294" s="11"/>
+      <c r="J293" s="11"/>
+    </row>
+    <row r="294" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E294" s="8"/>
       <c r="F294" s="7"/>
       <c r="G294" s="2" t="s">
         <v>383</v>
@@ -5067,28 +5318,10 @@
       <c r="I294" s="2">
         <v>1</v>
       </c>
+      <c r="J294" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="32">
-    <mergeCell ref="E289:E294"/>
-    <mergeCell ref="E271:E285"/>
-    <mergeCell ref="E286:E288"/>
-    <mergeCell ref="E254:E270"/>
-    <mergeCell ref="E244:E248"/>
-    <mergeCell ref="E249:E250"/>
-    <mergeCell ref="E251:E253"/>
-    <mergeCell ref="E154:E170"/>
-    <mergeCell ref="E174:E178"/>
-    <mergeCell ref="E179:E190"/>
-    <mergeCell ref="E191:E194"/>
-    <mergeCell ref="E242:E243"/>
-    <mergeCell ref="E195:E199"/>
-    <mergeCell ref="E171:E172"/>
-    <mergeCell ref="E201:E204"/>
-    <mergeCell ref="E205:E210"/>
-    <mergeCell ref="E211:E219"/>
-    <mergeCell ref="E220:E235"/>
-    <mergeCell ref="E236:E241"/>
     <mergeCell ref="E3:I4"/>
     <mergeCell ref="E130:E145"/>
     <mergeCell ref="E146:E153"/>
@@ -5102,10 +5335,29 @@
     <mergeCell ref="E111:E120"/>
     <mergeCell ref="E121:E128"/>
     <mergeCell ref="E88:E89"/>
+    <mergeCell ref="E154:E170"/>
+    <mergeCell ref="E174:E178"/>
+    <mergeCell ref="E179:E190"/>
+    <mergeCell ref="E191:E194"/>
+    <mergeCell ref="E242:E243"/>
+    <mergeCell ref="E195:E199"/>
+    <mergeCell ref="E171:E172"/>
+    <mergeCell ref="E201:E204"/>
+    <mergeCell ref="E205:E210"/>
+    <mergeCell ref="E211:E219"/>
+    <mergeCell ref="E220:E235"/>
+    <mergeCell ref="E236:E241"/>
+    <mergeCell ref="E289:E294"/>
+    <mergeCell ref="E271:E285"/>
+    <mergeCell ref="E286:E288"/>
+    <mergeCell ref="E254:E270"/>
+    <mergeCell ref="E244:E248"/>
+    <mergeCell ref="E249:E250"/>
+    <mergeCell ref="E251:E253"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" scale="85" fitToHeight="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="67" fitToHeight="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;"-,Bold"&amp;16I&amp;&amp;C STORE MANAGEMENT</oddHeader>
     <oddFooter xml:space="preserve">&amp;L&amp;D&amp;CINSTRUMENT &amp;&amp; CONTROL&amp;R&amp;P

</xml_diff>